<commit_message>
step 3 and 4 work
</commit_message>
<xml_diff>
--- a/Functions and Code/Color Palette.xlsx
+++ b/Functions and Code/Color Palette.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\matlabroot\Functions and Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Evyn\matlabroot\Functions and Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A059B237-3B65-4D4B-80A9-04C0B73A7114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203B5E85-4F64-43EA-BFBE-7A343039D16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9495" yWindow="750" windowWidth="34560" windowHeight="17595" xr2:uid="{B90EF345-F11D-4BE8-9704-8686C964E4D8}"/>
+    <workbookView xWindow="240" yWindow="795" windowWidth="27705" windowHeight="14010" xr2:uid="{B90EF345-F11D-4BE8-9704-8686C964E4D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="424">
   <si>
     <t>GreenYellow</t>
   </si>
@@ -3157,7 +3157,7 @@
   <dimension ref="A1:T158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3428,6 +3428,16 @@
         <v>324</v>
       </c>
       <c r="D14" s="58"/>
+      <c r="H14" s="139" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" s="139" t="s">
+        <v>80</v>
+      </c>
+      <c r="J14" s="173" t="s">
+        <v>325</v>
+      </c>
+      <c r="K14" s="59"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="139" t="s">
@@ -3440,6 +3450,16 @@
         <v>325</v>
       </c>
       <c r="D15" s="59"/>
+      <c r="H15" s="139" t="s">
+        <v>94</v>
+      </c>
+      <c r="I15" s="139" t="s">
+        <v>95</v>
+      </c>
+      <c r="J15" s="173" t="s">
+        <v>332</v>
+      </c>
+      <c r="K15" s="154"/>
     </row>
     <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="139" t="s">
@@ -3452,8 +3472,18 @@
         <v>326</v>
       </c>
       <c r="D16" s="60"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="139" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="139" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="173" t="s">
+        <v>365</v>
+      </c>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="139" t="s">
         <v>83</v>
       </c>
@@ -3464,8 +3494,18 @@
         <v>327</v>
       </c>
       <c r="D17" s="168"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="139" t="s">
+        <v>191</v>
+      </c>
+      <c r="I17" s="139" t="s">
+        <v>192</v>
+      </c>
+      <c r="J17" s="173" t="s">
+        <v>420</v>
+      </c>
+      <c r="K17" s="40"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="170" t="s">
         <v>85</v>
       </c>
@@ -3473,7 +3513,7 @@
       <c r="C18" s="175"/>
       <c r="D18" s="169"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="139" t="s">
         <v>86</v>
       </c>
@@ -3485,7 +3525,7 @@
       </c>
       <c r="D19" s="61"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="139" t="s">
         <v>88</v>
       </c>
@@ -3497,7 +3537,7 @@
       </c>
       <c r="D20" s="62"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="139" t="s">
         <v>90</v>
       </c>
@@ -3509,7 +3549,7 @@
       </c>
       <c r="D21" s="63"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="139" t="s">
         <v>92</v>
       </c>
@@ -3521,7 +3561,7 @@
       </c>
       <c r="D22" s="64"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="139" t="s">
         <v>94</v>
       </c>
@@ -3533,7 +3573,7 @@
       </c>
       <c r="D23" s="154"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="159" t="s">
         <v>96</v>
       </c>
@@ -3541,7 +3581,7 @@
       <c r="C24" s="176"/>
       <c r="D24" s="161"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="139" t="s">
         <v>97</v>
       </c>
@@ -3553,7 +3593,7 @@
       </c>
       <c r="D25" s="65"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="139" t="s">
         <v>99</v>
       </c>
@@ -3565,7 +3605,7 @@
       </c>
       <c r="D26" s="66"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="139" t="s">
         <v>101</v>
       </c>
@@ -3577,7 +3617,7 @@
       </c>
       <c r="D27" s="67"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="139" t="s">
         <v>103</v>
       </c>
@@ -3589,7 +3629,7 @@
       </c>
       <c r="D28" s="68"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="139" t="s">
         <v>105</v>
       </c>
@@ -3601,7 +3641,7 @@
       </c>
       <c r="D29" s="69"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="139" t="s">
         <v>107</v>
       </c>
@@ -3613,7 +3653,7 @@
       </c>
       <c r="D30" s="70"/>
     </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="139" t="s">
         <v>109</v>
       </c>
@@ -3625,7 +3665,7 @@
       </c>
       <c r="D31" s="71"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="139" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
NOAA and temp control
</commit_message>
<xml_diff>
--- a/Functions and Code/Color Palette.xlsx
+++ b/Functions and Code/Color Palette.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\matlabroot\Functions and Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Evyn\matlabroot\Functions and Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526ED565-5C80-45B9-BB1A-826DA9B28117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4DE018-3210-4382-9FA1-88CE688DF95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="21690" windowHeight="17595" xr2:uid="{B90EF345-F11D-4BE8-9704-8686C964E4D8}"/>
+    <workbookView xWindow="1680" yWindow="2010" windowWidth="21600" windowHeight="11385" xr2:uid="{B90EF345-F11D-4BE8-9704-8686C964E4D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="425">
   <si>
     <t>GreenYellow</t>
   </si>
@@ -1303,6 +1303,9 @@
   </si>
   <si>
     <t>Male</t>
+  </si>
+  <si>
+    <t>Temp Rate Colors:</t>
   </si>
 </sst>
 </file>
@@ -2286,7 +2289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2832,6 +2835,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="145" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -3157,8 +3163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBF5F8C-DD5F-4ED3-9E54-88EB7CF98784}">
   <dimension ref="A1:T158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="M54" sqref="M54"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3167,6 +3173,7 @@
     <col min="2" max="2" width="8.42578125" style="139" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" style="173" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" style="24" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.7109375" customWidth="1"/>
   </cols>
@@ -4019,7 +4026,7 @@
       </c>
       <c r="I48" s="83"/>
     </row>
-    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="139" t="s">
         <v>143</v>
       </c>
@@ -4035,7 +4042,7 @@
       </c>
       <c r="I49" s="59"/>
     </row>
-    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="139" t="s">
         <v>145</v>
       </c>
@@ -4051,7 +4058,7 @@
       </c>
       <c r="I50" s="154"/>
     </row>
-    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="139" t="s">
         <v>146</v>
       </c>
@@ -4067,7 +4074,7 @@
       </c>
       <c r="I51" s="4"/>
     </row>
-    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="139" t="s">
         <v>147</v>
       </c>
@@ -4083,7 +4090,7 @@
       </c>
       <c r="I52" s="40"/>
     </row>
-    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="139" t="s">
         <v>149</v>
       </c>
@@ -4099,7 +4106,7 @@
       </c>
       <c r="I53" s="23"/>
     </row>
-    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="139" t="s">
         <v>151</v>
       </c>
@@ -4115,7 +4122,7 @@
       </c>
       <c r="I54" s="54"/>
     </row>
-    <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="139" t="s">
         <v>153</v>
       </c>
@@ -4127,15 +4134,18 @@
       </c>
       <c r="D55" s="92"/>
     </row>
-    <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="150" t="s">
         <v>155</v>
       </c>
       <c r="B56" s="151"/>
       <c r="C56" s="178"/>
       <c r="D56" s="152"/>
-    </row>
-    <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H56" s="183" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="139" t="s">
         <v>0</v>
       </c>
@@ -4146,8 +4156,13 @@
         <v>362</v>
       </c>
       <c r="D57" s="1"/>
-    </row>
-    <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H57" s="139" t="s">
+        <v>167</v>
+      </c>
+      <c r="I57" s="29"/>
+      <c r="J57" s="173"/>
+    </row>
+    <row r="58" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="139" t="s">
         <v>2</v>
       </c>
@@ -4158,8 +4173,13 @@
         <v>363</v>
       </c>
       <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H58" s="139" t="s">
+        <v>139</v>
+      </c>
+      <c r="I58" s="84"/>
+      <c r="J58" s="173"/>
+    </row>
+    <row r="59" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="139" t="s">
         <v>4</v>
       </c>
@@ -4170,8 +4190,13 @@
         <v>364</v>
       </c>
       <c r="D59" s="3"/>
-    </row>
-    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H59" s="139" t="s">
+        <v>94</v>
+      </c>
+      <c r="I59" s="154"/>
+      <c r="J59" s="173"/>
+    </row>
+    <row r="60" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="139" t="s">
         <v>6</v>
       </c>
@@ -4183,7 +4208,7 @@
       </c>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="139" t="s">
         <v>8</v>
       </c>
@@ -4195,7 +4220,7 @@
       </c>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="139" t="s">
         <v>10</v>
       </c>
@@ -4207,7 +4232,7 @@
       </c>
       <c r="D62" s="6"/>
     </row>
-    <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="139" t="s">
         <v>12</v>
       </c>
@@ -4219,7 +4244,7 @@
       </c>
       <c r="D63" s="7"/>
     </row>
-    <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="139" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
poster data analysis updates
</commit_message>
<xml_diff>
--- a/Functions and Code/Color Palette.xlsx
+++ b/Functions and Code/Color Palette.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evynd\Documents\matlabroot\Functions and Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\matlabroot\Functions and Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D0CCDF-42E0-4784-82AF-51C93AC88703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D992B1-EE19-4E02-AC38-8413C6DA03BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{B90EF345-F11D-4BE8-9704-8686C964E4D8}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="32610" windowHeight="20985" xr2:uid="{B90EF345-F11D-4BE8-9704-8686C964E4D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -936,9 +936,6 @@
     <t>2F4F4F</t>
   </si>
   <si>
-    <t>47,79,79</t>
-  </si>
-  <si>
     <t>Black</t>
   </si>
   <si>
@@ -1306,6 +1303,9 @@
   </si>
   <si>
     <t>All comparisons Colors</t>
+  </si>
+  <si>
+    <t>49,49,49</t>
   </si>
 </sst>
 </file>
@@ -2207,12 +2207,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF2F4F4F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2232,6 +2226,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF313131"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2804,14 +2804,29 @@
     <xf numFmtId="0" fontId="3" fillId="142" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="143" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="26" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="118" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="143" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="143" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="143" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="134" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="144" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="144" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2819,24 +2834,6 @@
     <xf numFmtId="0" fontId="4" fillId="144" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="144" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="134" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="145" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="145" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="145" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="52" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2912,13 +2909,13 @@
     <xf numFmtId="0" fontId="3" fillId="70" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="146" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="146" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="145" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="145" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="146" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="145" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="50" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2930,7 +2927,7 @@
     <xf numFmtId="49" fontId="0" fillId="56" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="146" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="145" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="53" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2948,10 +2945,10 @@
     <xf numFmtId="49" fontId="0" fillId="52" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="143" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="144" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="145" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3000,7 +2997,10 @@
     <xf numFmtId="0" fontId="3" fillId="34" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="147" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="146" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="147" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3010,6 +3010,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF313131"/>
+      <color rgb="FF4F4F4F"/>
       <color rgb="FF410082"/>
       <color rgb="FFFF00FF"/>
     </mruColors>
@@ -3324,15 +3326,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBF5F8C-DD5F-4ED3-9E54-88EB7CF98784}">
   <dimension ref="A1:AF152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W77" sqref="W77:W89"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F146" sqref="F146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="172" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="171" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" style="24" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -3343,12 +3345,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="164" t="s">
-        <v>306</v>
-      </c>
-      <c r="B1" s="165"/>
-      <c r="C1" s="171"/>
-      <c r="D1" s="166"/>
+      <c r="A1" s="163" t="s">
+        <v>305</v>
+      </c>
+      <c r="B1" s="164"/>
+      <c r="C1" s="170"/>
+      <c r="D1" s="165"/>
     </row>
     <row r="2" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
@@ -3357,8 +3359,8 @@
       <c r="B2" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="172" t="s">
-        <v>307</v>
+      <c r="C2" s="171" t="s">
+        <v>306</v>
       </c>
       <c r="D2" s="48"/>
     </row>
@@ -3369,8 +3371,8 @@
       <c r="B3" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="172" t="s">
-        <v>308</v>
+      <c r="C3" s="171" t="s">
+        <v>307</v>
       </c>
       <c r="D3" s="49"/>
     </row>
@@ -3381,8 +3383,8 @@
       <c r="B4" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="172" t="s">
-        <v>309</v>
+      <c r="C4" s="171" t="s">
+        <v>308</v>
       </c>
       <c r="D4" s="50"/>
     </row>
@@ -3393,8 +3395,8 @@
       <c r="B5" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="172" t="s">
-        <v>310</v>
+      <c r="C5" s="171" t="s">
+        <v>309</v>
       </c>
       <c r="D5" s="51"/>
     </row>
@@ -3405,12 +3407,12 @@
       <c r="B6" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="172" t="s">
-        <v>311</v>
+      <c r="C6" s="171" t="s">
+        <v>310</v>
       </c>
       <c r="D6" s="52"/>
       <c r="H6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I6" s="24" t="s">
         <v>253</v>
@@ -3418,8 +3420,8 @@
       <c r="J6" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="K6" s="172" t="s">
-        <v>389</v>
+      <c r="K6" s="171" t="s">
+        <v>388</v>
       </c>
       <c r="L6" s="88"/>
       <c r="M6" s="24" t="s">
@@ -3428,8 +3430,8 @@
       <c r="N6" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="O6" s="172" t="s">
-        <v>330</v>
+      <c r="O6" s="171" t="s">
+        <v>329</v>
       </c>
       <c r="P6" s="68"/>
       <c r="Q6" s="24" t="s">
@@ -3438,8 +3440,8 @@
       <c r="R6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="S6" s="172" t="s">
-        <v>361</v>
+      <c r="S6" s="171" t="s">
+        <v>360</v>
       </c>
       <c r="T6" s="6"/>
     </row>
@@ -3450,12 +3452,12 @@
       <c r="B7" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="172" t="s">
-        <v>312</v>
+      <c r="C7" s="171" t="s">
+        <v>311</v>
       </c>
       <c r="D7" s="53"/>
       <c r="H7" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I7" s="24" t="s">
         <v>290</v>
@@ -3463,8 +3465,8 @@
       <c r="J7" s="24" t="s">
         <v>291</v>
       </c>
-      <c r="K7" s="172" t="s">
-        <v>407</v>
+      <c r="K7" s="171" t="s">
+        <v>406</v>
       </c>
       <c r="L7" s="125"/>
       <c r="M7" s="24" t="s">
@@ -3473,8 +3475,8 @@
       <c r="N7" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="O7" s="172" t="s">
-        <v>327</v>
+      <c r="O7" s="171" t="s">
+        <v>326</v>
       </c>
       <c r="P7" s="65"/>
       <c r="Q7" s="24" t="s">
@@ -3483,8 +3485,8 @@
       <c r="R7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="S7" s="172" t="s">
-        <v>363</v>
+      <c r="S7" s="171" t="s">
+        <v>362</v>
       </c>
       <c r="T7" s="10"/>
     </row>
@@ -3495,12 +3497,12 @@
       <c r="B8" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="172" t="s">
-        <v>313</v>
+      <c r="C8" s="171" t="s">
+        <v>312</v>
       </c>
       <c r="D8" s="54"/>
       <c r="H8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I8" s="24" t="s">
         <v>297</v>
@@ -3508,8 +3510,8 @@
       <c r="J8" s="24">
         <v>808080</v>
       </c>
-      <c r="K8" s="172" t="s">
-        <v>410</v>
+      <c r="K8" s="171" t="s">
+        <v>409</v>
       </c>
       <c r="L8" s="128"/>
       <c r="M8" s="24" t="s">
@@ -3518,8 +3520,8 @@
       <c r="N8" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="O8" s="172" t="s">
-        <v>325</v>
+      <c r="O8" s="171" t="s">
+        <v>324</v>
       </c>
       <c r="P8" s="64"/>
       <c r="Q8" s="24" t="s">
@@ -3528,7 +3530,7 @@
       <c r="R8" s="24">
         <v>6400</v>
       </c>
-      <c r="S8" s="172" t="s">
+      <c r="S8" s="171" t="s">
         <v>31</v>
       </c>
       <c r="T8" s="14"/>
@@ -3540,8 +3542,8 @@
       <c r="B9" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="172" t="s">
-        <v>314</v>
+      <c r="C9" s="171" t="s">
+        <v>313</v>
       </c>
       <c r="D9" s="55"/>
     </row>
@@ -3552,26 +3554,26 @@
       <c r="B10" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="172" t="s">
-        <v>315</v>
-      </c>
-      <c r="D10" s="154"/>
-      <c r="AB10" s="198"/>
-      <c r="AC10" s="198"/>
-      <c r="AD10" s="198"/>
-      <c r="AE10" s="198"/>
+      <c r="C10" s="171" t="s">
+        <v>314</v>
+      </c>
+      <c r="D10" s="153"/>
+      <c r="AB10" s="197"/>
+      <c r="AC10" s="197"/>
+      <c r="AD10" s="197"/>
+      <c r="AE10" s="197"/>
     </row>
     <row r="11" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="161" t="s">
+      <c r="A11" s="160" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="162"/>
-      <c r="C11" s="173"/>
-      <c r="D11" s="163"/>
-      <c r="AB11" s="198"/>
-      <c r="AC11" s="198"/>
-      <c r="AD11" s="198"/>
-      <c r="AE11" s="198"/>
+      <c r="B11" s="161"/>
+      <c r="C11" s="172"/>
+      <c r="D11" s="162"/>
+      <c r="AB11" s="197"/>
+      <c r="AC11" s="197"/>
+      <c r="AD11" s="197"/>
+      <c r="AE11" s="197"/>
     </row>
     <row r="12" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
@@ -3580,14 +3582,14 @@
       <c r="B12" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="172" t="s">
-        <v>316</v>
+      <c r="C12" s="171" t="s">
+        <v>315</v>
       </c>
       <c r="D12" s="56"/>
-      <c r="AB12" s="198"/>
-      <c r="AC12" s="198"/>
-      <c r="AD12" s="198"/>
-      <c r="AE12" s="198"/>
+      <c r="AB12" s="197"/>
+      <c r="AC12" s="197"/>
+      <c r="AD12" s="197"/>
+      <c r="AE12" s="197"/>
     </row>
     <row r="13" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -3596,14 +3598,14 @@
       <c r="B13" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="172" t="s">
-        <v>317</v>
+      <c r="C13" s="171" t="s">
+        <v>316</v>
       </c>
       <c r="D13" s="57"/>
-      <c r="AB13" s="198"/>
-      <c r="AC13" s="198"/>
-      <c r="AD13" s="198"/>
-      <c r="AE13" s="198"/>
+      <c r="AB13" s="197"/>
+      <c r="AC13" s="197"/>
+      <c r="AD13" s="197"/>
+      <c r="AE13" s="197"/>
     </row>
     <row r="14" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -3612,8 +3614,8 @@
       <c r="B14" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="172" t="s">
-        <v>318</v>
+      <c r="C14" s="171" t="s">
+        <v>317</v>
       </c>
       <c r="D14" s="58"/>
       <c r="H14" s="24" t="s">
@@ -3622,17 +3624,17 @@
       <c r="I14" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="J14" s="172" t="s">
-        <v>319</v>
+      <c r="J14" s="171" t="s">
+        <v>318</v>
       </c>
       <c r="K14" s="59"/>
       <c r="Z14" s="24" t="s">
         <v>253</v>
       </c>
-      <c r="AB14" s="198"/>
-      <c r="AC14" s="198"/>
+      <c r="AB14" s="197"/>
+      <c r="AC14" s="197"/>
       <c r="AD14" s="130"/>
-      <c r="AE14" s="198"/>
+      <c r="AE14" s="197"/>
       <c r="AF14" s="24" t="s">
         <v>299</v>
       </c>
@@ -3644,8 +3646,8 @@
       <c r="B15" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="172" t="s">
-        <v>319</v>
+      <c r="C15" s="171" t="s">
+        <v>318</v>
       </c>
       <c r="D15" s="59"/>
       <c r="H15" s="24" t="s">
@@ -3654,19 +3656,19 @@
       <c r="I15" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="J15" s="172" t="s">
-        <v>326</v>
-      </c>
-      <c r="K15" s="153"/>
+      <c r="J15" s="171" t="s">
+        <v>325</v>
+      </c>
+      <c r="K15" s="152"/>
       <c r="Z15" s="24" t="s">
         <v>297</v>
       </c>
-      <c r="AB15" s="198"/>
-      <c r="AC15" s="198"/>
+      <c r="AB15" s="197"/>
+      <c r="AC15" s="197"/>
       <c r="AD15" s="88"/>
-      <c r="AE15" s="198"/>
+      <c r="AE15" s="197"/>
       <c r="AF15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="16" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3676,8 +3678,8 @@
       <c r="B16" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="172" t="s">
-        <v>320</v>
+      <c r="C16" s="171" t="s">
+        <v>319</v>
       </c>
       <c r="D16" s="60"/>
       <c r="H16" s="24" t="s">
@@ -3686,17 +3688,17 @@
       <c r="I16" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="J16" s="172" t="s">
-        <v>359</v>
+      <c r="J16" s="171" t="s">
+        <v>358</v>
       </c>
       <c r="K16" s="4"/>
       <c r="Z16" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="AB16" s="198"/>
-      <c r="AC16" s="198"/>
+      <c r="AB16" s="197"/>
+      <c r="AC16" s="197"/>
       <c r="AD16" s="57"/>
-      <c r="AE16" s="198"/>
+      <c r="AE16" s="197"/>
       <c r="AF16" s="24" t="s">
         <v>75</v>
       </c>
@@ -3708,18 +3710,18 @@
       <c r="B17" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="172" t="s">
-        <v>321</v>
-      </c>
-      <c r="D17" s="167"/>
+      <c r="C17" s="171" t="s">
+        <v>320</v>
+      </c>
+      <c r="D17" s="166"/>
       <c r="H17" s="24" t="s">
         <v>191</v>
       </c>
       <c r="I17" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="J17" s="172" t="s">
-        <v>414</v>
+      <c r="J17" s="171" t="s">
+        <v>413</v>
       </c>
       <c r="K17" s="40"/>
       <c r="M17" s="24" t="s">
@@ -3728,35 +3730,35 @@
       <c r="N17" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="O17" s="172" t="s">
-        <v>367</v>
+      <c r="O17" s="171" t="s">
+        <v>366</v>
       </c>
       <c r="P17" s="26"/>
       <c r="Z17" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="AB17" s="198"/>
-      <c r="AC17" s="198"/>
+      <c r="AB17" s="197"/>
+      <c r="AC17" s="197"/>
       <c r="AD17" s="59"/>
-      <c r="AE17" s="198"/>
+      <c r="AE17" s="197"/>
       <c r="AF17" s="24" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="169" t="s">
+      <c r="A18" s="168" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="170"/>
-      <c r="C18" s="174"/>
-      <c r="D18" s="168"/>
+      <c r="B18" s="169"/>
+      <c r="C18" s="173"/>
+      <c r="D18" s="167"/>
       <c r="M18" s="24" t="s">
         <v>160</v>
       </c>
       <c r="N18" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="O18" s="172" t="s">
+      <c r="O18" s="171" t="s">
         <v>159</v>
       </c>
       <c r="P18" s="25"/>
@@ -3768,10 +3770,10 @@
         <v>122</v>
       </c>
       <c r="X18" s="76"/>
-      <c r="AB18" s="198"/>
-      <c r="AC18" s="198"/>
-      <c r="AD18" s="198"/>
-      <c r="AE18" s="198"/>
+      <c r="AB18" s="197"/>
+      <c r="AC18" s="197"/>
+      <c r="AD18" s="197"/>
+      <c r="AE18" s="197"/>
     </row>
     <row r="19" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
@@ -3780,8 +3782,8 @@
       <c r="B19" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="172" t="s">
-        <v>322</v>
+      <c r="C19" s="171" t="s">
+        <v>321</v>
       </c>
       <c r="D19" s="61"/>
       <c r="M19" s="24" t="s">
@@ -3790,8 +3792,8 @@
       <c r="N19" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="O19" s="172" t="s">
-        <v>414</v>
+      <c r="O19" s="171" t="s">
+        <v>413</v>
       </c>
       <c r="P19" s="40"/>
       <c r="S19" s="24" t="s">
@@ -3802,10 +3804,10 @@
         <v>137</v>
       </c>
       <c r="X19" s="83"/>
-      <c r="AB19" s="198"/>
-      <c r="AC19" s="198"/>
-      <c r="AD19" s="198"/>
-      <c r="AE19" s="198"/>
+      <c r="AB19" s="197"/>
+      <c r="AC19" s="197"/>
+      <c r="AD19" s="197"/>
+      <c r="AE19" s="197"/>
     </row>
     <row r="20" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
@@ -3814,8 +3816,8 @@
       <c r="B20" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="172" t="s">
-        <v>323</v>
+      <c r="C20" s="171" t="s">
+        <v>322</v>
       </c>
       <c r="D20" s="62"/>
       <c r="M20" s="24" t="s">
@@ -3824,7 +3826,7 @@
       <c r="N20" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="O20" s="172" t="s">
+      <c r="O20" s="171" t="s">
         <v>204</v>
       </c>
       <c r="P20" s="45"/>
@@ -3836,10 +3838,10 @@
         <v>10</v>
       </c>
       <c r="X20" s="6"/>
-      <c r="AB20" s="198"/>
-      <c r="AC20" s="198"/>
-      <c r="AD20" s="198"/>
-      <c r="AE20" s="198"/>
+      <c r="AB20" s="197"/>
+      <c r="AC20" s="197"/>
+      <c r="AD20" s="197"/>
+      <c r="AE20" s="197"/>
     </row>
     <row r="21" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
@@ -3848,8 +3850,8 @@
       <c r="B21" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="172" t="s">
-        <v>324</v>
+      <c r="C21" s="171" t="s">
+        <v>323</v>
       </c>
       <c r="D21" s="63"/>
       <c r="H21" s="24" t="s">
@@ -3858,8 +3860,8 @@
       <c r="I21" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="J21" s="172" t="s">
-        <v>317</v>
+      <c r="J21" s="171" t="s">
+        <v>316</v>
       </c>
       <c r="K21" s="57"/>
       <c r="W21" s="24" t="s">
@@ -3867,12 +3869,12 @@
       </c>
       <c r="X21" s="13"/>
       <c r="Z21" t="s">
-        <v>424</v>
-      </c>
-      <c r="AB21" s="198"/>
-      <c r="AC21" s="198"/>
-      <c r="AD21" s="198"/>
-      <c r="AE21" s="198"/>
+        <v>423</v>
+      </c>
+      <c r="AB21" s="197"/>
+      <c r="AC21" s="197"/>
+      <c r="AD21" s="197"/>
+      <c r="AE21" s="197"/>
     </row>
     <row r="22" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
@@ -3881,8 +3883,8 @@
       <c r="B22" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="C22" s="172" t="s">
-        <v>325</v>
+      <c r="C22" s="171" t="s">
+        <v>324</v>
       </c>
       <c r="D22" s="64"/>
       <c r="H22" s="24" t="s">
@@ -3891,14 +3893,14 @@
       <c r="I22" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="J22" s="172" t="s">
-        <v>319</v>
+      <c r="J22" s="171" t="s">
+        <v>318</v>
       </c>
       <c r="K22" s="59"/>
-      <c r="AB22" s="198"/>
-      <c r="AC22" s="198"/>
-      <c r="AD22" s="198"/>
-      <c r="AE22" s="198"/>
+      <c r="AB22" s="197"/>
+      <c r="AC22" s="197"/>
+      <c r="AD22" s="197"/>
+      <c r="AE22" s="197"/>
     </row>
     <row r="23" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
@@ -3907,48 +3909,48 @@
       <c r="B23" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="172" t="s">
-        <v>326</v>
-      </c>
-      <c r="D23" s="153"/>
+      <c r="C23" s="171" t="s">
+        <v>325</v>
+      </c>
+      <c r="D23" s="152"/>
       <c r="H23" s="24" t="s">
         <v>191</v>
       </c>
       <c r="I23" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="J23" s="172" t="s">
-        <v>414</v>
+      <c r="J23" s="171" t="s">
+        <v>413</v>
       </c>
       <c r="K23" s="40"/>
       <c r="M23" s="24"/>
       <c r="N23" s="24"/>
-      <c r="O23" s="172"/>
+      <c r="O23" s="171"/>
       <c r="P23" s="24" t="s">
         <v>75</v>
       </c>
       <c r="Q23" s="57"/>
     </row>
     <row r="24" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="158" t="s">
+      <c r="A24" s="157" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="159"/>
-      <c r="C24" s="175"/>
-      <c r="D24" s="160"/>
+      <c r="B24" s="158"/>
+      <c r="C24" s="174"/>
+      <c r="D24" s="159"/>
       <c r="H24" s="24" t="s">
         <v>186</v>
       </c>
       <c r="I24" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="J24" s="172" t="s">
-        <v>378</v>
+      <c r="J24" s="171" t="s">
+        <v>377</v>
       </c>
       <c r="K24" s="38"/>
       <c r="M24" s="24"/>
       <c r="N24" s="24"/>
-      <c r="O24" s="172"/>
+      <c r="O24" s="171"/>
       <c r="P24" s="24" t="s">
         <v>186</v>
       </c>
@@ -3961,13 +3963,13 @@
       <c r="B25" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="C25" s="172" t="s">
-        <v>327</v>
+      <c r="C25" s="171" t="s">
+        <v>326</v>
       </c>
       <c r="D25" s="65"/>
       <c r="M25" s="24"/>
       <c r="N25" s="24"/>
-      <c r="O25" s="172"/>
+      <c r="O25" s="171"/>
       <c r="P25" s="24" t="s">
         <v>10</v>
       </c>
@@ -3980,13 +3982,13 @@
       <c r="B26" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="172" t="s">
-        <v>328</v>
+      <c r="C26" s="171" t="s">
+        <v>327</v>
       </c>
       <c r="D26" s="66"/>
       <c r="M26" s="24"/>
       <c r="N26" s="24"/>
-      <c r="O26" s="172"/>
+      <c r="O26" s="171"/>
     </row>
     <row r="27" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
@@ -3995,8 +3997,8 @@
       <c r="B27" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="C27" s="172" t="s">
-        <v>329</v>
+      <c r="C27" s="171" t="s">
+        <v>328</v>
       </c>
       <c r="D27" s="67"/>
       <c r="H27" s="24" t="s">
@@ -4011,8 +4013,8 @@
       <c r="B28" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="172" t="s">
-        <v>330</v>
+      <c r="C28" s="171" t="s">
+        <v>329</v>
       </c>
       <c r="D28" s="68"/>
       <c r="H28" s="24" t="s">
@@ -4025,8 +4027,8 @@
       <c r="AA28" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="AB28" s="172" t="s">
-        <v>359</v>
+      <c r="AB28" s="171" t="s">
+        <v>358</v>
       </c>
       <c r="AC28" s="4"/>
     </row>
@@ -4037,8 +4039,8 @@
       <c r="B29" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="C29" s="172" t="s">
-        <v>331</v>
+      <c r="C29" s="171" t="s">
+        <v>330</v>
       </c>
       <c r="D29" s="69"/>
       <c r="H29" s="24" t="s">
@@ -4053,8 +4055,8 @@
       <c r="B30" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="172" t="s">
-        <v>332</v>
+      <c r="C30" s="171" t="s">
+        <v>331</v>
       </c>
       <c r="D30" s="70"/>
       <c r="H30" s="24" t="s">
@@ -4069,8 +4071,8 @@
       <c r="B31" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="C31" s="172" t="s">
-        <v>333</v>
+      <c r="C31" s="171" t="s">
+        <v>332</v>
       </c>
       <c r="D31" s="71"/>
     </row>
@@ -4081,8 +4083,8 @@
       <c r="B32" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="C32" s="172" t="s">
-        <v>334</v>
+      <c r="C32" s="171" t="s">
+        <v>333</v>
       </c>
       <c r="D32" s="72"/>
       <c r="Y32" s="24" t="s">
@@ -4097,8 +4099,8 @@
       <c r="B33" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="C33" s="172" t="s">
-        <v>335</v>
+      <c r="C33" s="171" t="s">
+        <v>334</v>
       </c>
       <c r="D33" s="73"/>
       <c r="Y33" s="24" t="s">
@@ -4113,8 +4115,8 @@
       <c r="B34" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="C34" s="172" t="s">
-        <v>336</v>
+      <c r="C34" s="171" t="s">
+        <v>335</v>
       </c>
       <c r="D34" s="74"/>
       <c r="Y34" s="24" t="s">
@@ -4129,15 +4131,15 @@
       <c r="B35" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="C35" s="172" t="s">
-        <v>337</v>
-      </c>
-      <c r="D35" s="152"/>
+      <c r="C35" s="171" t="s">
+        <v>336</v>
+      </c>
+      <c r="D35" s="151"/>
       <c r="I35" s="24" t="s">
         <v>120</v>
       </c>
       <c r="J35" s="75"/>
-      <c r="K35" s="172"/>
+      <c r="K35" s="171"/>
       <c r="O35" s="24" t="s">
         <v>120</v>
       </c>
@@ -4148,12 +4150,12 @@
       <c r="Z35" s="28"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="155" t="s">
+      <c r="A36" s="154" t="s">
         <v>119</v>
       </c>
-      <c r="B36" s="156"/>
-      <c r="C36" s="176"/>
-      <c r="D36" s="157"/>
+      <c r="B36" s="155"/>
+      <c r="C36" s="175"/>
+      <c r="D36" s="156"/>
       <c r="I36" s="24" t="s">
         <v>122</v>
       </c>
@@ -4174,8 +4176,8 @@
       <c r="B37" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="C37" s="172" t="s">
-        <v>338</v>
+      <c r="C37" s="171" t="s">
+        <v>337</v>
       </c>
       <c r="D37" s="75"/>
       <c r="I37" s="24" t="s">
@@ -4198,8 +4200,8 @@
       <c r="B38" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="C38" s="172" t="s">
-        <v>339</v>
+      <c r="C38" s="171" t="s">
+        <v>338</v>
       </c>
       <c r="D38" s="76"/>
       <c r="I38" s="24" t="s">
@@ -4222,8 +4224,8 @@
       <c r="B39" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="C39" s="172" t="s">
-        <v>340</v>
+      <c r="C39" s="171" t="s">
+        <v>339</v>
       </c>
       <c r="D39" s="77"/>
       <c r="I39" s="24" t="s">
@@ -4246,8 +4248,8 @@
       <c r="B40" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C40" s="172" t="s">
-        <v>341</v>
+      <c r="C40" s="171" t="s">
+        <v>340</v>
       </c>
       <c r="D40" s="78"/>
       <c r="I40" s="24" t="s">
@@ -4266,8 +4268,8 @@
       <c r="B41" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="C41" s="172" t="s">
-        <v>342</v>
+      <c r="C41" s="171" t="s">
+        <v>341</v>
       </c>
       <c r="D41" s="79"/>
       <c r="I41" s="24" t="s">
@@ -4282,8 +4284,8 @@
       <c r="B42" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C42" s="172" t="s">
-        <v>343</v>
+      <c r="C42" s="171" t="s">
+        <v>342</v>
       </c>
       <c r="D42" s="80"/>
     </row>
@@ -4294,8 +4296,8 @@
       <c r="B43" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C43" s="172" t="s">
-        <v>343</v>
+      <c r="C43" s="171" t="s">
+        <v>342</v>
       </c>
       <c r="D43" s="80"/>
     </row>
@@ -4306,8 +4308,8 @@
       <c r="B44" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="C44" s="172" t="s">
-        <v>344</v>
+      <c r="C44" s="171" t="s">
+        <v>343</v>
       </c>
       <c r="D44" s="81"/>
     </row>
@@ -4318,8 +4320,8 @@
       <c r="B45" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="C45" s="172" t="s">
-        <v>345</v>
+      <c r="C45" s="171" t="s">
+        <v>344</v>
       </c>
       <c r="D45" s="82"/>
     </row>
@@ -4330,8 +4332,8 @@
       <c r="B46" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="C46" s="172" t="s">
-        <v>346</v>
+      <c r="C46" s="171" t="s">
+        <v>345</v>
       </c>
       <c r="D46" s="83"/>
     </row>
@@ -4342,11 +4344,11 @@
       <c r="B47" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="C47" s="172" t="s">
-        <v>347</v>
+      <c r="C47" s="171" t="s">
+        <v>346</v>
       </c>
       <c r="D47" s="84"/>
-      <c r="J47" s="172"/>
+      <c r="J47" s="171"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
@@ -4355,8 +4357,8 @@
       <c r="B48" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="C48" s="172" t="s">
-        <v>348</v>
+      <c r="C48" s="171" t="s">
+        <v>347</v>
       </c>
       <c r="D48" s="85"/>
       <c r="H48" s="24" t="s">
@@ -4375,8 +4377,8 @@
       <c r="B49" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="C49" s="172" t="s">
-        <v>349</v>
+      <c r="C49" s="171" t="s">
+        <v>348</v>
       </c>
       <c r="D49" s="86"/>
       <c r="H49" s="24" t="s">
@@ -4395,14 +4397,14 @@
       <c r="B50" s="24">
         <v>800080</v>
       </c>
-      <c r="C50" s="172" t="s">
-        <v>350</v>
+      <c r="C50" s="171" t="s">
+        <v>349</v>
       </c>
       <c r="D50" s="87"/>
       <c r="H50" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="I50" s="153"/>
+      <c r="I50" s="152"/>
       <c r="K50" s="24" t="s">
         <v>124</v>
       </c>
@@ -4415,8 +4417,8 @@
       <c r="B51" s="24">
         <v>663399</v>
       </c>
-      <c r="C51" s="172" t="s">
-        <v>351</v>
+      <c r="C51" s="171" t="s">
+        <v>350</v>
       </c>
       <c r="D51" s="88"/>
       <c r="H51" s="24" t="s">
@@ -4435,8 +4437,8 @@
       <c r="B52" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="C52" s="172" t="s">
-        <v>352</v>
+      <c r="C52" s="171" t="s">
+        <v>351</v>
       </c>
       <c r="D52" s="89"/>
       <c r="H52" s="24" t="s">
@@ -4451,8 +4453,8 @@
       <c r="B53" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="C53" s="172" t="s">
-        <v>353</v>
+      <c r="C53" s="171" t="s">
+        <v>352</v>
       </c>
       <c r="D53" s="90"/>
       <c r="H53" s="24" t="s">
@@ -4471,8 +4473,8 @@
       <c r="B54" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="C54" s="172" t="s">
-        <v>354</v>
+      <c r="C54" s="171" t="s">
+        <v>353</v>
       </c>
       <c r="D54" s="91"/>
       <c r="H54" s="24" t="s">
@@ -4491,8 +4493,8 @@
       <c r="B55" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="C55" s="172" t="s">
-        <v>355</v>
+      <c r="C55" s="171" t="s">
+        <v>354</v>
       </c>
       <c r="D55" s="92"/>
       <c r="H55" s="24" t="s">
@@ -4503,21 +4505,21 @@
         <v>165</v>
       </c>
       <c r="L55" s="28"/>
-      <c r="M55" s="172"/>
+      <c r="M55" s="171"/>
     </row>
     <row r="56" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="149" t="s">
+      <c r="A56" s="148" t="s">
         <v>155</v>
       </c>
-      <c r="B56" s="150"/>
-      <c r="C56" s="177"/>
-      <c r="D56" s="151"/>
+      <c r="B56" s="149"/>
+      <c r="C56" s="176"/>
+      <c r="D56" s="150"/>
       <c r="H56" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="I56" s="154"/>
+      <c r="I56" s="153"/>
       <c r="K56" s="24"/>
-      <c r="M56" s="172"/>
+      <c r="M56" s="171"/>
     </row>
     <row r="57" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="24" t="s">
@@ -4526,8 +4528,8 @@
       <c r="B57" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C57" s="172" t="s">
-        <v>356</v>
+      <c r="C57" s="171" t="s">
+        <v>355</v>
       </c>
       <c r="D57" s="1"/>
       <c r="H57" s="24" t="s">
@@ -4550,8 +4552,8 @@
       <c r="B58" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C58" s="172" t="s">
-        <v>357</v>
+      <c r="C58" s="171" t="s">
+        <v>356</v>
       </c>
       <c r="D58" s="2"/>
       <c r="H58" s="24" t="s">
@@ -4561,12 +4563,12 @@
       <c r="K58" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="L58" s="154"/>
+      <c r="L58" s="153"/>
       <c r="P58" s="24" t="s">
         <v>30</v>
       </c>
       <c r="Q58" s="14"/>
-      <c r="R58" s="172"/>
+      <c r="R58" s="171"/>
     </row>
     <row r="59" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="24" t="s">
@@ -4575,8 +4577,8 @@
       <c r="B59" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="172" t="s">
-        <v>358</v>
+      <c r="C59" s="171" t="s">
+        <v>357</v>
       </c>
       <c r="D59" s="3"/>
       <c r="P59" s="24" t="s">
@@ -4595,17 +4597,17 @@
       <c r="B60" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C60" s="172" t="s">
-        <v>359</v>
+      <c r="C60" s="171" t="s">
+        <v>358</v>
       </c>
       <c r="D60" s="4"/>
-      <c r="H60" s="182" t="s">
-        <v>418</v>
+      <c r="H60" s="181" t="s">
+        <v>417</v>
       </c>
       <c r="K60" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="L60" s="153"/>
+      <c r="L60" s="152"/>
       <c r="P60" s="24" t="s">
         <v>147</v>
       </c>
@@ -4622,22 +4624,22 @@
       <c r="B61" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C61" s="172" t="s">
-        <v>360</v>
+      <c r="C61" s="171" t="s">
+        <v>359</v>
       </c>
       <c r="D61" s="5"/>
       <c r="H61" s="24" t="s">
         <v>167</v>
       </c>
       <c r="I61" s="29"/>
-      <c r="J61" s="183" t="s">
-        <v>419</v>
+      <c r="J61" s="182" t="s">
+        <v>418</v>
       </c>
       <c r="K61" s="24" t="s">
         <v>97</v>
       </c>
       <c r="L61" s="65"/>
-      <c r="M61" s="172"/>
+      <c r="M61" s="171"/>
       <c r="P61" s="24" t="s">
         <v>79</v>
       </c>
@@ -4654,16 +4656,16 @@
       <c r="B62" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C62" s="172" t="s">
-        <v>361</v>
+      <c r="C62" s="171" t="s">
+        <v>360</v>
       </c>
       <c r="D62" s="6"/>
       <c r="H62" s="24" t="s">
         <v>139</v>
       </c>
       <c r="I62" s="84"/>
-      <c r="J62" s="183" t="s">
-        <v>421</v>
+      <c r="J62" s="182" t="s">
+        <v>420</v>
       </c>
       <c r="P62" s="24" t="s">
         <v>97</v>
@@ -4681,18 +4683,18 @@
       <c r="B63" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C63" s="172" t="s">
-        <v>362</v>
+      <c r="C63" s="171" t="s">
+        <v>361</v>
       </c>
       <c r="D63" s="7"/>
       <c r="H63" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="I63" s="153"/>
-      <c r="J63" s="183" t="s">
-        <v>420</v>
-      </c>
-      <c r="R63" s="172"/>
+      <c r="I63" s="152"/>
+      <c r="J63" s="182" t="s">
+        <v>419</v>
+      </c>
+      <c r="R63" s="171"/>
     </row>
     <row r="64" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="24" t="s">
@@ -4701,7 +4703,7 @@
       <c r="B64" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C64" s="172" t="s">
+      <c r="C64" s="171" t="s">
         <v>16</v>
       </c>
       <c r="D64" s="8"/>
@@ -4709,7 +4711,7 @@
         <v>191</v>
       </c>
       <c r="I64" s="40"/>
-      <c r="J64" s="184">
+      <c r="J64" s="183">
         <v>0.16</v>
       </c>
     </row>
@@ -4720,7 +4722,7 @@
       <c r="B65" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C65" s="172" t="s">
+      <c r="C65" s="171" t="s">
         <v>19</v>
       </c>
       <c r="D65" s="9"/>
@@ -4736,15 +4738,15 @@
       <c r="B66" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C66" s="172" t="s">
-        <v>363</v>
+      <c r="C66" s="171" t="s">
+        <v>362</v>
       </c>
       <c r="D66" s="10"/>
       <c r="H66" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="I66" s="154"/>
-      <c r="J66" s="172"/>
+      <c r="I66" s="153"/>
+      <c r="J66" s="171"/>
       <c r="N66" s="24" t="s">
         <v>139</v>
       </c>
@@ -4757,7 +4759,7 @@
       <c r="B67" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C67" s="172" t="s">
+      <c r="C67" s="171" t="s">
         <v>24</v>
       </c>
       <c r="D67" s="11"/>
@@ -4765,11 +4767,11 @@
         <v>147</v>
       </c>
       <c r="I67" s="89"/>
-      <c r="J67" s="172"/>
+      <c r="J67" s="171"/>
       <c r="N67" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="O67" s="153"/>
+      <c r="O67" s="152"/>
     </row>
     <row r="68" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="24" t="s">
@@ -4778,7 +4780,7 @@
       <c r="B68" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C68" s="172" t="s">
+      <c r="C68" s="171" t="s">
         <v>27</v>
       </c>
       <c r="D68" s="12"/>
@@ -4786,7 +4788,7 @@
         <v>52</v>
       </c>
       <c r="I68" s="23"/>
-      <c r="J68" s="172"/>
+      <c r="J68" s="171"/>
       <c r="N68" s="24" t="s">
         <v>97</v>
       </c>
@@ -4803,7 +4805,7 @@
       <c r="B69" s="24">
         <v>8000</v>
       </c>
-      <c r="C69" s="172" t="s">
+      <c r="C69" s="171" t="s">
         <v>29</v>
       </c>
       <c r="D69" s="13"/>
@@ -4811,8 +4813,8 @@
         <v>196</v>
       </c>
       <c r="O69" s="43"/>
-      <c r="Q69" s="185" t="s">
-        <v>422</v>
+      <c r="Q69" s="184" t="s">
+        <v>421</v>
       </c>
       <c r="U69" s="24" t="s">
         <v>128</v>
@@ -4829,7 +4831,7 @@
       <c r="B70" s="24">
         <v>6400</v>
       </c>
-      <c r="C70" s="172" t="s">
+      <c r="C70" s="171" t="s">
         <v>31</v>
       </c>
       <c r="D70" s="14"/>
@@ -4837,7 +4839,7 @@
         <v>191</v>
       </c>
       <c r="O70" s="40"/>
-      <c r="P70" s="172"/>
+      <c r="P70" s="171"/>
       <c r="Q70" t="s">
         <v>161</v>
       </c>
@@ -4857,7 +4859,7 @@
       <c r="B71" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C71" s="172" t="s">
+      <c r="C71" s="171" t="s">
         <v>34</v>
       </c>
       <c r="D71" s="15"/>
@@ -4876,7 +4878,7 @@
       <c r="B72" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C72" s="172" t="s">
+      <c r="C72" s="171" t="s">
         <v>37</v>
       </c>
       <c r="D72" s="16"/>
@@ -4899,14 +4901,14 @@
       <c r="B73" s="24">
         <v>808000</v>
       </c>
-      <c r="C73" s="172" t="s">
+      <c r="C73" s="171" t="s">
         <v>39</v>
       </c>
       <c r="D73" s="17"/>
       <c r="Q73" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="R73" s="153"/>
+      <c r="R73" s="152"/>
       <c r="U73" s="24" t="s">
         <v>188</v>
       </c>
@@ -4922,7 +4924,7 @@
       <c r="B74" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C74" s="172" t="s">
+      <c r="C74" s="171" t="s">
         <v>42</v>
       </c>
       <c r="D74" s="18"/>
@@ -4945,8 +4947,8 @@
       <c r="B75" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C75" s="172" t="s">
-        <v>364</v>
+      <c r="C75" s="171" t="s">
+        <v>363</v>
       </c>
       <c r="D75" s="19"/>
       <c r="Q75" s="24" t="s">
@@ -4961,8 +4963,8 @@
       <c r="B76" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C76" s="172" t="s">
-        <v>365</v>
+      <c r="C76" s="171" t="s">
+        <v>364</v>
       </c>
       <c r="D76" s="20"/>
       <c r="K76" s="24" t="s">
@@ -4973,8 +4975,8 @@
         <v>99</v>
       </c>
       <c r="R76" s="66"/>
-      <c r="T76" s="185" t="s">
-        <v>426</v>
+      <c r="T76" s="184" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="77" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4984,8 +4986,8 @@
       <c r="B77" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C77" s="172" t="s">
-        <v>366</v>
+      <c r="C77" s="171" t="s">
+        <v>365</v>
       </c>
       <c r="D77" s="21"/>
       <c r="K77" s="24" t="s">
@@ -5008,14 +5010,14 @@
       <c r="B78" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C78" s="172" t="s">
+      <c r="C78" s="171" t="s">
         <v>51</v>
       </c>
       <c r="D78" s="22"/>
       <c r="K78" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="L78" s="153"/>
+      <c r="L78" s="152"/>
       <c r="Q78" s="24" t="s">
         <v>66</v>
       </c>
@@ -5032,7 +5034,7 @@
       <c r="B79" s="24">
         <v>8080</v>
       </c>
-      <c r="C79" s="172" t="s">
+      <c r="C79" s="171" t="s">
         <v>53</v>
       </c>
       <c r="D79" s="23"/>
@@ -5046,12 +5048,12 @@
       <c r="X79" s="80"/>
     </row>
     <row r="80" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="146" t="s">
+      <c r="A80" s="145" t="s">
         <v>156</v>
       </c>
-      <c r="B80" s="147"/>
-      <c r="C80" s="178"/>
-      <c r="D80" s="148"/>
+      <c r="B80" s="146"/>
+      <c r="C80" s="177"/>
+      <c r="D80" s="147"/>
       <c r="Q80" s="24" t="s">
         <v>261</v>
       </c>
@@ -5072,7 +5074,7 @@
       <c r="B81" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="C81" s="172" t="s">
+      <c r="C81" s="171" t="s">
         <v>159</v>
       </c>
       <c r="D81" s="25"/>
@@ -5095,7 +5097,7 @@
       <c r="B82" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="C82" s="172" t="s">
+      <c r="C82" s="171" t="s">
         <v>159</v>
       </c>
       <c r="D82" s="25"/>
@@ -5105,8 +5107,8 @@
       <c r="L82" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="M82" s="172" t="s">
-        <v>313</v>
+      <c r="M82" s="171" t="s">
+        <v>312</v>
       </c>
       <c r="N82" s="54"/>
       <c r="Q82" s="24" t="s">
@@ -5116,7 +5118,7 @@
       <c r="W82" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="X82" s="153"/>
+      <c r="X82" s="152"/>
     </row>
     <row r="83" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="24" t="s">
@@ -5125,14 +5127,14 @@
       <c r="B83" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="C83" s="172" t="s">
-        <v>367</v>
+      <c r="C83" s="171" t="s">
+        <v>366</v>
       </c>
       <c r="D83" s="26"/>
       <c r="K83" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="M83" s="172" t="s">
+      <c r="M83" s="171" t="s">
         <v>190</v>
       </c>
       <c r="N83" s="39"/>
@@ -5152,8 +5154,8 @@
       <c r="B84" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="C84" s="172" t="s">
-        <v>368</v>
+      <c r="C84" s="171" t="s">
+        <v>367</v>
       </c>
       <c r="D84" s="27"/>
       <c r="Q84" s="24" t="s">
@@ -5176,8 +5178,8 @@
       <c r="B85" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="C85" s="172" t="s">
-        <v>369</v>
+      <c r="C85" s="171" t="s">
+        <v>368</v>
       </c>
       <c r="D85" s="28"/>
       <c r="Q85" s="24" t="s">
@@ -5196,8 +5198,8 @@
       <c r="B86" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="C86" s="172" t="s">
-        <v>370</v>
+      <c r="C86" s="171" t="s">
+        <v>369</v>
       </c>
       <c r="D86" s="29"/>
       <c r="Q86" s="24" t="s">
@@ -5220,8 +5222,8 @@
       <c r="B87" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="C87" s="172" t="s">
-        <v>371</v>
+      <c r="C87" s="171" t="s">
+        <v>370</v>
       </c>
       <c r="D87" s="30"/>
       <c r="Q87" s="24" t="s">
@@ -5244,7 +5246,7 @@
       <c r="B88" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="C88" s="172" t="s">
+      <c r="C88" s="171" t="s">
         <v>173</v>
       </c>
       <c r="D88" s="31"/>
@@ -5260,8 +5262,8 @@
       <c r="B89" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="C89" s="172" t="s">
-        <v>372</v>
+      <c r="C89" s="171" t="s">
+        <v>371</v>
       </c>
       <c r="D89" s="32"/>
       <c r="W89" s="24" t="s">
@@ -5276,8 +5278,8 @@
       <c r="B90" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="C90" s="172" t="s">
-        <v>373</v>
+      <c r="C90" s="171" t="s">
+        <v>372</v>
       </c>
       <c r="D90" s="33"/>
     </row>
@@ -5288,8 +5290,8 @@
       <c r="B91" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="C91" s="172" t="s">
-        <v>374</v>
+      <c r="C91" s="171" t="s">
+        <v>373</v>
       </c>
       <c r="D91" s="34"/>
     </row>
@@ -5300,8 +5302,8 @@
       <c r="B92" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="C92" s="172" t="s">
-        <v>375</v>
+      <c r="C92" s="171" t="s">
+        <v>374</v>
       </c>
       <c r="D92" s="35"/>
     </row>
@@ -5312,8 +5314,8 @@
       <c r="B93" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="C93" s="172" t="s">
-        <v>376</v>
+      <c r="C93" s="171" t="s">
+        <v>375</v>
       </c>
       <c r="D93" s="36"/>
     </row>
@@ -5324,8 +5326,8 @@
       <c r="B94" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="C94" s="172" t="s">
-        <v>377</v>
+      <c r="C94" s="171" t="s">
+        <v>376</v>
       </c>
       <c r="D94" s="37"/>
     </row>
@@ -5336,8 +5338,8 @@
       <c r="B95" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="C95" s="172" t="s">
-        <v>378</v>
+      <c r="C95" s="171" t="s">
+        <v>377</v>
       </c>
       <c r="D95" s="38"/>
     </row>
@@ -5348,7 +5350,7 @@
       <c r="B96" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="C96" s="172" t="s">
+      <c r="C96" s="171" t="s">
         <v>190</v>
       </c>
       <c r="D96" s="39"/>
@@ -5360,8 +5362,8 @@
       <c r="B97" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="C97" s="172" t="s">
-        <v>414</v>
+      <c r="C97" s="171" t="s">
+        <v>413</v>
       </c>
       <c r="D97" s="40"/>
     </row>
@@ -5372,62 +5374,62 @@
       <c r="B98" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="C98" s="172" t="s">
-        <v>379</v>
+      <c r="C98" s="171" t="s">
+        <v>378</v>
       </c>
       <c r="D98" s="41"/>
-      <c r="J98" s="186" t="s">
+      <c r="J98" s="185" t="s">
         <v>253</v>
       </c>
-      <c r="K98" s="187" t="s">
+      <c r="K98" s="186" t="s">
         <v>254</v>
       </c>
-      <c r="L98" s="188" t="s">
-        <v>389</v>
-      </c>
-      <c r="M98" s="193"/>
-      <c r="N98" s="186" t="s">
+      <c r="L98" s="187" t="s">
+        <v>388</v>
+      </c>
+      <c r="M98" s="192"/>
+      <c r="N98" s="185" t="s">
         <v>292</v>
       </c>
-      <c r="O98" s="187" t="s">
+      <c r="O98" s="186" t="s">
         <v>291</v>
       </c>
-      <c r="P98" s="188" t="s">
-        <v>407</v>
-      </c>
-      <c r="Q98" s="196"/>
+      <c r="P98" s="187" t="s">
+        <v>406</v>
+      </c>
+      <c r="Q98" s="195"/>
     </row>
     <row r="99" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="B99" s="139">
+      <c r="B99" s="138">
         <v>41690</v>
       </c>
-      <c r="C99" s="172" t="s">
-        <v>380</v>
+      <c r="C99" s="171" t="s">
+        <v>379</v>
       </c>
       <c r="D99" s="42"/>
-      <c r="J99" s="189" t="s">
+      <c r="J99" s="188" t="s">
         <v>188</v>
       </c>
       <c r="K99" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="L99" s="172" t="s">
+      <c r="L99" s="171" t="s">
         <v>190</v>
       </c>
-      <c r="M99" s="194"/>
-      <c r="N99" s="189" t="s">
+      <c r="M99" s="193"/>
+      <c r="N99" s="188" t="s">
         <v>174</v>
       </c>
       <c r="O99" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="P99" s="172" t="s">
-        <v>372</v>
-      </c>
-      <c r="Q99" s="197"/>
+      <c r="P99" s="171" t="s">
+        <v>371</v>
+      </c>
+      <c r="Q99" s="196"/>
     </row>
     <row r="100" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="24" t="s">
@@ -5436,30 +5438,30 @@
       <c r="B100" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="C100" s="172" t="s">
+      <c r="C100" s="171" t="s">
         <v>198</v>
       </c>
       <c r="D100" s="43"/>
-      <c r="J100" s="190" t="s">
+      <c r="J100" s="189" t="s">
         <v>196</v>
       </c>
-      <c r="K100" s="191" t="s">
+      <c r="K100" s="190" t="s">
         <v>197</v>
       </c>
-      <c r="L100" s="192" t="s">
+      <c r="L100" s="191" t="s">
         <v>198</v>
       </c>
-      <c r="M100" s="195"/>
-      <c r="N100" s="190" t="s">
+      <c r="M100" s="194"/>
+      <c r="N100" s="189" t="s">
         <v>196</v>
       </c>
-      <c r="O100" s="191" t="s">
+      <c r="O100" s="190" t="s">
         <v>197</v>
       </c>
-      <c r="P100" s="192" t="s">
+      <c r="P100" s="191" t="s">
         <v>198</v>
       </c>
-      <c r="Q100" s="195"/>
+      <c r="Q100" s="194"/>
     </row>
     <row r="101" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="24" t="s">
@@ -5468,7 +5470,7 @@
       <c r="B101" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="C101" s="172" t="s">
+      <c r="C101" s="171" t="s">
         <v>201</v>
       </c>
       <c r="D101" s="44"/>
@@ -5480,7 +5482,7 @@
       <c r="B102" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="C102" s="172" t="s">
+      <c r="C102" s="171" t="s">
         <v>204</v>
       </c>
       <c r="D102" s="45"/>
@@ -5492,7 +5494,7 @@
       <c r="B103" s="24">
         <v>80</v>
       </c>
-      <c r="C103" s="172" t="s">
+      <c r="C103" s="171" t="s">
         <v>206</v>
       </c>
       <c r="D103" s="46"/>
@@ -5504,18 +5506,18 @@
       <c r="B104" s="24">
         <v>191970</v>
       </c>
-      <c r="C104" s="172" t="s">
+      <c r="C104" s="171" t="s">
         <v>208</v>
       </c>
       <c r="D104" s="47"/>
     </row>
     <row r="105" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="143" t="s">
+      <c r="A105" s="142" t="s">
         <v>209</v>
       </c>
-      <c r="B105" s="144"/>
-      <c r="C105" s="179"/>
-      <c r="D105" s="145"/>
+      <c r="B105" s="143"/>
+      <c r="C105" s="178"/>
+      <c r="D105" s="144"/>
     </row>
     <row r="106" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="24" t="s">
@@ -5524,8 +5526,8 @@
       <c r="B106" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="C106" s="172" t="s">
-        <v>381</v>
+      <c r="C106" s="171" t="s">
+        <v>380</v>
       </c>
       <c r="D106" s="93"/>
     </row>
@@ -5536,8 +5538,8 @@
       <c r="B107" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="C107" s="172" t="s">
-        <v>382</v>
+      <c r="C107" s="171" t="s">
+        <v>381</v>
       </c>
       <c r="D107" s="94"/>
     </row>
@@ -5548,8 +5550,8 @@
       <c r="B108" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="C108" s="172" t="s">
-        <v>383</v>
+      <c r="C108" s="171" t="s">
+        <v>382</v>
       </c>
       <c r="D108" s="95"/>
     </row>
@@ -5560,8 +5562,8 @@
       <c r="B109" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="C109" s="172" t="s">
-        <v>384</v>
+      <c r="C109" s="171" t="s">
+        <v>383</v>
       </c>
       <c r="D109" s="96"/>
     </row>
@@ -5572,8 +5574,8 @@
       <c r="B110" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="C110" s="172" t="s">
-        <v>385</v>
+      <c r="C110" s="171" t="s">
+        <v>384</v>
       </c>
       <c r="D110" s="97"/>
     </row>
@@ -5584,8 +5586,8 @@
       <c r="B111" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="C111" s="172" t="s">
-        <v>386</v>
+      <c r="C111" s="171" t="s">
+        <v>385</v>
       </c>
       <c r="D111" s="98"/>
     </row>
@@ -5596,8 +5598,8 @@
       <c r="B112" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="C112" s="172" t="s">
-        <v>387</v>
+      <c r="C112" s="171" t="s">
+        <v>386</v>
       </c>
       <c r="D112" s="99"/>
     </row>
@@ -5608,8 +5610,8 @@
       <c r="B113" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="C113" s="172" t="s">
-        <v>388</v>
+      <c r="C113" s="171" t="s">
+        <v>387</v>
       </c>
       <c r="D113" s="100"/>
       <c r="J113" s="24" t="s">
@@ -5624,7 +5626,7 @@
       <c r="B114" s="24" t="s">
         <v>227</v>
       </c>
-      <c r="C114" s="172" t="s">
+      <c r="C114" s="171" t="s">
         <v>228</v>
       </c>
       <c r="D114" s="101"/>
@@ -5636,7 +5638,7 @@
       <c r="B115" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="C115" s="172" t="s">
+      <c r="C115" s="171" t="s">
         <v>231</v>
       </c>
       <c r="D115" s="102"/>
@@ -5648,7 +5650,7 @@
       <c r="B116" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="C116" s="172" t="s">
+      <c r="C116" s="171" t="s">
         <v>234</v>
       </c>
       <c r="D116" s="103"/>
@@ -5660,7 +5662,7 @@
       <c r="B117" s="24" t="s">
         <v>236</v>
       </c>
-      <c r="C117" s="172" t="s">
+      <c r="C117" s="171" t="s">
         <v>237</v>
       </c>
       <c r="D117" s="104"/>
@@ -5672,7 +5674,7 @@
       <c r="B118" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="C118" s="172" t="s">
+      <c r="C118" s="171" t="s">
         <v>240</v>
       </c>
       <c r="D118" s="105"/>
@@ -5684,7 +5686,7 @@
       <c r="B119" s="24" t="s">
         <v>242</v>
       </c>
-      <c r="C119" s="172" t="s">
+      <c r="C119" s="171" t="s">
         <v>243</v>
       </c>
       <c r="D119" s="106"/>
@@ -5696,7 +5698,7 @@
       <c r="B120" s="24" t="s">
         <v>245</v>
       </c>
-      <c r="C120" s="172" t="s">
+      <c r="C120" s="171" t="s">
         <v>246</v>
       </c>
       <c r="D120" s="107"/>
@@ -5708,12 +5710,12 @@
       <c r="B121" s="24" t="s">
         <v>248</v>
       </c>
-      <c r="C121" s="172" t="s">
+      <c r="C121" s="171" t="s">
         <v>249</v>
       </c>
       <c r="D121" s="108"/>
-      <c r="H121" s="185" t="s">
-        <v>423</v>
+      <c r="H121" s="184" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="122" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5723,36 +5725,36 @@
       <c r="B122" s="24">
         <v>800000</v>
       </c>
-      <c r="C122" s="172" t="s">
+      <c r="C122" s="171" t="s">
         <v>251</v>
       </c>
-      <c r="D122" s="134"/>
+      <c r="D122" s="133"/>
       <c r="H122" s="24" t="s">
         <v>66</v>
       </c>
       <c r="I122" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="J122" s="172" t="s">
-        <v>313</v>
+      <c r="J122" s="171" t="s">
+        <v>312</v>
       </c>
       <c r="K122" s="54"/>
     </row>
     <row r="123" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="137" t="s">
+      <c r="A123" s="136" t="s">
         <v>252</v>
       </c>
-      <c r="B123" s="135"/>
-      <c r="C123" s="180"/>
-      <c r="D123" s="136"/>
+      <c r="B123" s="134"/>
+      <c r="C123" s="179"/>
+      <c r="D123" s="135"/>
       <c r="H123" s="24" t="s">
         <v>97</v>
       </c>
       <c r="I123" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="J123" s="172" t="s">
-        <v>327</v>
+      <c r="J123" s="171" t="s">
+        <v>326</v>
       </c>
       <c r="K123" s="65"/>
     </row>
@@ -5763,8 +5765,8 @@
       <c r="B124" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="C124" s="172" t="s">
-        <v>389</v>
+      <c r="C124" s="171" t="s">
+        <v>388</v>
       </c>
       <c r="D124" s="88"/>
       <c r="H124" s="24" t="s">
@@ -5773,8 +5775,8 @@
       <c r="I124" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="J124" s="172" t="s">
-        <v>348</v>
+      <c r="J124" s="171" t="s">
+        <v>347</v>
       </c>
       <c r="K124" s="85"/>
     </row>
@@ -5785,8 +5787,8 @@
       <c r="B125" s="24" t="s">
         <v>256</v>
       </c>
-      <c r="C125" s="172" t="s">
-        <v>390</v>
+      <c r="C125" s="171" t="s">
+        <v>389</v>
       </c>
       <c r="D125" s="109"/>
       <c r="H125" s="24" t="s">
@@ -5795,8 +5797,8 @@
       <c r="I125" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="J125" s="172" t="s">
-        <v>360</v>
+      <c r="J125" s="171" t="s">
+        <v>359</v>
       </c>
       <c r="K125" s="5"/>
     </row>
@@ -5807,8 +5809,8 @@
       <c r="B126" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="C126" s="172" t="s">
-        <v>391</v>
+      <c r="C126" s="171" t="s">
+        <v>390</v>
       </c>
       <c r="D126" s="110"/>
       <c r="H126" s="24" t="s">
@@ -5817,7 +5819,7 @@
       <c r="I126" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="J126" s="172" t="s">
+      <c r="J126" s="171" t="s">
         <v>190</v>
       </c>
       <c r="K126" s="39"/>
@@ -5829,8 +5831,8 @@
       <c r="B127" s="24" t="s">
         <v>260</v>
       </c>
-      <c r="C127" s="172" t="s">
-        <v>392</v>
+      <c r="C127" s="171" t="s">
+        <v>391</v>
       </c>
       <c r="D127" s="111"/>
       <c r="H127" s="24" t="s">
@@ -5839,8 +5841,8 @@
       <c r="I127" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="J127" s="172" t="s">
-        <v>389</v>
+      <c r="J127" s="171" t="s">
+        <v>388</v>
       </c>
       <c r="K127" s="88"/>
     </row>
@@ -5851,8 +5853,8 @@
       <c r="B128" s="24" t="s">
         <v>262</v>
       </c>
-      <c r="C128" s="172" t="s">
-        <v>393</v>
+      <c r="C128" s="171" t="s">
+        <v>392</v>
       </c>
       <c r="D128" s="112"/>
       <c r="H128" s="24" t="s">
@@ -5861,7 +5863,7 @@
       <c r="I128" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="J128" s="172" t="s">
+      <c r="J128" s="171" t="s">
         <v>198</v>
       </c>
       <c r="K128" s="43"/>
@@ -5873,8 +5875,8 @@
       <c r="B129" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="C129" s="172" t="s">
-        <v>394</v>
+      <c r="C129" s="171" t="s">
+        <v>393</v>
       </c>
       <c r="D129" s="113"/>
       <c r="H129" s="24" t="s">
@@ -5883,8 +5885,8 @@
       <c r="I129" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="J129" s="172" t="s">
-        <v>319</v>
+      <c r="J129" s="171" t="s">
+        <v>318</v>
       </c>
       <c r="K129" s="59"/>
     </row>
@@ -5895,8 +5897,8 @@
       <c r="B130" s="24" t="s">
         <v>266</v>
       </c>
-      <c r="C130" s="172" t="s">
-        <v>395</v>
+      <c r="C130" s="171" t="s">
+        <v>394</v>
       </c>
       <c r="D130" s="114"/>
       <c r="H130" s="24" t="s">
@@ -5905,8 +5907,8 @@
       <c r="I130" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="J130" s="172" t="s">
-        <v>311</v>
+      <c r="J130" s="171" t="s">
+        <v>310</v>
       </c>
       <c r="K130" s="52"/>
     </row>
@@ -5917,8 +5919,8 @@
       <c r="B131" s="24" t="s">
         <v>268</v>
       </c>
-      <c r="C131" s="172" t="s">
-        <v>396</v>
+      <c r="C131" s="171" t="s">
+        <v>395</v>
       </c>
       <c r="D131" s="115"/>
     </row>
@@ -5929,8 +5931,8 @@
       <c r="B132" s="24" t="s">
         <v>270</v>
       </c>
-      <c r="C132" s="172" t="s">
-        <v>397</v>
+      <c r="C132" s="171" t="s">
+        <v>396</v>
       </c>
       <c r="D132" s="116"/>
     </row>
@@ -5941,8 +5943,8 @@
       <c r="B133" s="24" t="s">
         <v>272</v>
       </c>
-      <c r="C133" s="172" t="s">
-        <v>398</v>
+      <c r="C133" s="171" t="s">
+        <v>397</v>
       </c>
       <c r="D133" s="117"/>
     </row>
@@ -5953,8 +5955,8 @@
       <c r="B134" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="C134" s="172" t="s">
-        <v>399</v>
+      <c r="C134" s="171" t="s">
+        <v>398</v>
       </c>
       <c r="D134" s="118"/>
     </row>
@@ -5965,8 +5967,8 @@
       <c r="B135" s="24" t="s">
         <v>276</v>
       </c>
-      <c r="C135" s="172" t="s">
-        <v>400</v>
+      <c r="C135" s="171" t="s">
+        <v>399</v>
       </c>
       <c r="D135" s="119"/>
     </row>
@@ -5977,8 +5979,8 @@
       <c r="B136" s="24" t="s">
         <v>278</v>
       </c>
-      <c r="C136" s="172" t="s">
-        <v>401</v>
+      <c r="C136" s="171" t="s">
+        <v>400</v>
       </c>
       <c r="D136" s="120"/>
     </row>
@@ -5989,8 +5991,8 @@
       <c r="B137" s="24" t="s">
         <v>280</v>
       </c>
-      <c r="C137" s="172" t="s">
-        <v>402</v>
+      <c r="C137" s="171" t="s">
+        <v>401</v>
       </c>
       <c r="D137" s="121"/>
     </row>
@@ -6001,8 +6003,8 @@
       <c r="B138" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="C138" s="172" t="s">
-        <v>403</v>
+      <c r="C138" s="171" t="s">
+        <v>402</v>
       </c>
       <c r="D138" s="122"/>
     </row>
@@ -6013,8 +6015,8 @@
       <c r="B139" s="24" t="s">
         <v>284</v>
       </c>
-      <c r="C139" s="172" t="s">
-        <v>404</v>
+      <c r="C139" s="171" t="s">
+        <v>403</v>
       </c>
       <c r="D139" s="123"/>
     </row>
@@ -6025,18 +6027,18 @@
       <c r="B140" s="24" t="s">
         <v>286</v>
       </c>
-      <c r="C140" s="172" t="s">
-        <v>405</v>
-      </c>
-      <c r="D140" s="138"/>
+      <c r="C140" s="171" t="s">
+        <v>404</v>
+      </c>
+      <c r="D140" s="137"/>
     </row>
     <row r="141" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="140" t="s">
+      <c r="A141" s="139" t="s">
         <v>287</v>
       </c>
-      <c r="B141" s="141"/>
-      <c r="C141" s="181"/>
-      <c r="D141" s="142"/>
+      <c r="B141" s="140"/>
+      <c r="C141" s="180"/>
+      <c r="D141" s="141"/>
     </row>
     <row r="142" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="24" t="s">
@@ -6045,8 +6047,8 @@
       <c r="B142" s="24" t="s">
         <v>289</v>
       </c>
-      <c r="C142" s="172" t="s">
-        <v>406</v>
+      <c r="C142" s="171" t="s">
+        <v>405</v>
       </c>
       <c r="D142" s="124"/>
     </row>
@@ -6057,8 +6059,8 @@
       <c r="B143" s="24" t="s">
         <v>291</v>
       </c>
-      <c r="C143" s="172" t="s">
-        <v>407</v>
+      <c r="C143" s="171" t="s">
+        <v>406</v>
       </c>
       <c r="D143" s="125"/>
     </row>
@@ -6069,106 +6071,122 @@
       <c r="B144" s="24" t="s">
         <v>291</v>
       </c>
-      <c r="C144" s="172" t="s">
-        <v>407</v>
+      <c r="C144" s="171" t="s">
+        <v>406</v>
       </c>
       <c r="D144" s="125"/>
     </row>
-    <row r="145" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="24" t="s">
         <v>293</v>
       </c>
       <c r="B145" s="24" t="s">
         <v>294</v>
       </c>
-      <c r="C145" s="172" t="s">
-        <v>408</v>
+      <c r="C145" s="171" t="s">
+        <v>407</v>
       </c>
       <c r="D145" s="126"/>
     </row>
-    <row r="146" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="24" t="s">
         <v>295</v>
       </c>
       <c r="B146" s="24" t="s">
         <v>296</v>
       </c>
-      <c r="C146" s="172" t="s">
-        <v>409</v>
+      <c r="C146" s="171" t="s">
+        <v>408</v>
       </c>
       <c r="D146" s="127"/>
-    </row>
-    <row r="147" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J146" s="24"/>
+      <c r="K146" s="24"/>
+      <c r="L146" s="171"/>
+      <c r="M146" s="127"/>
+    </row>
+    <row r="147" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="24" t="s">
         <v>297</v>
       </c>
       <c r="B147" s="24">
         <v>808080</v>
       </c>
-      <c r="C147" s="172" t="s">
-        <v>410</v>
+      <c r="C147" s="171" t="s">
+        <v>409</v>
       </c>
       <c r="D147" s="128"/>
-    </row>
-    <row r="148" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J147" s="24"/>
+      <c r="K147" s="24"/>
+      <c r="L147" s="171"/>
+      <c r="M147" s="129"/>
+    </row>
+    <row r="148" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="24" t="s">
         <v>298</v>
       </c>
       <c r="B148" s="24">
         <v>696969</v>
       </c>
-      <c r="C148" s="172" t="s">
-        <v>411</v>
+      <c r="C148" s="171" t="s">
+        <v>410</v>
       </c>
       <c r="D148" s="129"/>
-    </row>
-    <row r="149" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J148" s="24"/>
+      <c r="K148" s="24"/>
+      <c r="L148" s="171"/>
+      <c r="M148" s="198"/>
+    </row>
+    <row r="149" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="24" t="s">
         <v>299</v>
       </c>
       <c r="B149" s="24">
         <v>778899</v>
       </c>
-      <c r="C149" s="172" t="s">
-        <v>412</v>
+      <c r="C149" s="171" t="s">
+        <v>411</v>
       </c>
       <c r="D149" s="130"/>
-    </row>
-    <row r="150" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J149" s="24"/>
+      <c r="K149" s="24"/>
+      <c r="L149" s="171"/>
+      <c r="M149" s="132"/>
+    </row>
+    <row r="150" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="24" t="s">
         <v>300</v>
       </c>
       <c r="B150" s="24">
         <v>708090</v>
       </c>
-      <c r="C150" s="172" t="s">
-        <v>413</v>
+      <c r="C150" s="171" t="s">
+        <v>412</v>
       </c>
       <c r="D150" s="131"/>
     </row>
-    <row r="151" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="24" t="s">
         <v>301</v>
       </c>
       <c r="B151" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="C151" s="172" t="s">
+      <c r="C151" s="171" t="s">
+        <v>426</v>
+      </c>
+      <c r="D151" s="198"/>
+    </row>
+    <row r="152" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="24" t="s">
         <v>303</v>
-      </c>
-      <c r="D151" s="132"/>
-    </row>
-    <row r="152" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="24" t="s">
-        <v>304</v>
       </c>
       <c r="B152" s="24">
         <v>0</v>
       </c>
-      <c r="C152" s="172" t="s">
-        <v>305</v>
-      </c>
-      <c r="D152" s="133"/>
+      <c r="C152" s="171" t="s">
+        <v>304</v>
+      </c>
+      <c r="D152" s="132"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
data processing for DPR figure updates
</commit_message>
<xml_diff>
--- a/Functions and Code/Color Palette.xlsx
+++ b/Functions and Code/Color Palette.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\matlabroot\Functions and Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evynd\Documents\matlabroot\Functions and Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2E687D-981D-4F78-96A8-D795B8FD726A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317C5E78-1CAC-41AD-A122-4DE0E85DE297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{B90EF345-F11D-4BE8-9704-8686C964E4D8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="427">
   <si>
     <t>GreenYellow</t>
   </si>
@@ -3324,10 +3324,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBF5F8C-DD5F-4ED3-9E54-88EB7CF98784}">
-  <dimension ref="A1:AF152"/>
+  <dimension ref="A1:AH152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T40" sqref="T40:T45"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF39" sqref="AF39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3703,7 +3703,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>83</v>
       </c>
@@ -3745,7 +3745,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="168" t="s">
         <v>85</v>
       </c>
@@ -3775,7 +3775,7 @@
       <c r="AD18" s="197"/>
       <c r="AE18" s="197"/>
     </row>
-    <row r="19" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
         <v>86</v>
       </c>
@@ -3809,7 +3809,7 @@
       <c r="AD19" s="197"/>
       <c r="AE19" s="197"/>
     </row>
-    <row r="20" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
         <v>88</v>
       </c>
@@ -3843,7 +3843,7 @@
       <c r="AD20" s="197"/>
       <c r="AE20" s="197"/>
     </row>
-    <row r="21" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>90</v>
       </c>
@@ -3876,7 +3876,7 @@
       <c r="AD21" s="197"/>
       <c r="AE21" s="197"/>
     </row>
-    <row r="22" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>92</v>
       </c>
@@ -3902,7 +3902,7 @@
       <c r="AD22" s="197"/>
       <c r="AE22" s="197"/>
     </row>
-    <row r="23" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>94</v>
       </c>
@@ -3931,7 +3931,7 @@
       </c>
       <c r="Q23" s="57"/>
     </row>
-    <row r="24" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="157" t="s">
         <v>96</v>
       </c>
@@ -3956,7 +3956,7 @@
       </c>
       <c r="Q24" s="38"/>
     </row>
-    <row r="25" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>97</v>
       </c>
@@ -3975,7 +3975,7 @@
       </c>
       <c r="Q25" s="6"/>
     </row>
-    <row r="26" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
         <v>99</v>
       </c>
@@ -3990,7 +3990,7 @@
       <c r="N26" s="24"/>
       <c r="O26" s="171"/>
     </row>
-    <row r="27" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
         <v>101</v>
       </c>
@@ -4006,7 +4006,7 @@
       </c>
       <c r="I27" s="62"/>
     </row>
-    <row r="28" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
         <v>103</v>
       </c>
@@ -4032,7 +4032,7 @@
       </c>
       <c r="AC28" s="4"/>
     </row>
-    <row r="29" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
         <v>105</v>
       </c>
@@ -4048,7 +4048,7 @@
       </c>
       <c r="I29" s="35"/>
     </row>
-    <row r="30" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="s">
         <v>107</v>
       </c>
@@ -4064,7 +4064,7 @@
       </c>
       <c r="I30" s="40"/>
     </row>
-    <row r="31" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="s">
         <v>109</v>
       </c>
@@ -4076,7 +4076,7 @@
       </c>
       <c r="D31" s="71"/>
     </row>
-    <row r="32" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>111</v>
       </c>
@@ -4094,8 +4094,18 @@
         <v>75</v>
       </c>
       <c r="Z32" s="57"/>
-    </row>
-    <row r="33" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE32" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF32" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG32" s="171" t="s">
+        <v>316</v>
+      </c>
+      <c r="AH32" s="57"/>
+    </row>
+    <row r="33" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="24" t="s">
         <v>113</v>
       </c>
@@ -4113,8 +4123,18 @@
         <v>79</v>
       </c>
       <c r="Z33" s="59"/>
-    </row>
-    <row r="34" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE33" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF33" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG33" s="171" t="s">
+        <v>317</v>
+      </c>
+      <c r="AH33" s="58"/>
+    </row>
+    <row r="34" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>115</v>
       </c>
@@ -4132,8 +4152,18 @@
         <v>52</v>
       </c>
       <c r="Z34" s="23"/>
-    </row>
-    <row r="35" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE34" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF34" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="AG34" s="171" t="s">
+        <v>413</v>
+      </c>
+      <c r="AH34" s="40"/>
+    </row>
+    <row r="35" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="24" t="s">
         <v>117</v>
       </c>
@@ -4161,7 +4191,7 @@
       </c>
       <c r="Z35" s="28"/>
     </row>
-    <row r="36" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="154" t="s">
         <v>119</v>
       </c>
@@ -4184,7 +4214,7 @@
       <c r="V36" s="43"/>
       <c r="W36" s="197"/>
     </row>
-    <row r="37" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="24" t="s">
         <v>120</v>
       </c>
@@ -4211,7 +4241,7 @@
       <c r="V37" s="197"/>
       <c r="W37" s="197"/>
     </row>
-    <row r="38" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="24" t="s">
         <v>122</v>
       </c>
@@ -4235,7 +4265,7 @@
       </c>
       <c r="P38" s="82"/>
     </row>
-    <row r="39" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="24" t="s">
         <v>124</v>
       </c>
@@ -4259,7 +4289,7 @@
       </c>
       <c r="P39" s="83"/>
     </row>
-    <row r="40" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="24" t="s">
         <v>126</v>
       </c>
@@ -4283,7 +4313,7 @@
       </c>
       <c r="U40" s="77"/>
     </row>
-    <row r="41" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="24" t="s">
         <v>128</v>
       </c>
@@ -4303,7 +4333,7 @@
       </c>
       <c r="U41" s="82"/>
     </row>
-    <row r="42" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="24" t="s">
         <v>130</v>
       </c>
@@ -4319,7 +4349,7 @@
       </c>
       <c r="U42" s="83"/>
     </row>
-    <row r="43" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="24" t="s">
         <v>132</v>
       </c>
@@ -4336,7 +4366,7 @@
       <c r="U43" s="38"/>
       <c r="V43" s="171"/>
     </row>
-    <row r="44" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="24" t="s">
         <v>133</v>
       </c>
@@ -4353,7 +4383,7 @@
       <c r="U44" s="40"/>
       <c r="V44" s="171"/>
     </row>
-    <row r="45" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="24" t="s">
         <v>135</v>
       </c>
@@ -4370,7 +4400,7 @@
       <c r="U45" s="43"/>
       <c r="V45" s="171"/>
     </row>
-    <row r="46" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="24" t="s">
         <v>137</v>
       </c>
@@ -4382,7 +4412,7 @@
       </c>
       <c r="D46" s="83"/>
     </row>
-    <row r="47" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="24" t="s">
         <v>139</v>
       </c>
@@ -4395,7 +4425,7 @@
       <c r="D47" s="84"/>
       <c r="J47" s="171"/>
     </row>
-    <row r="48" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
         <v>141</v>
       </c>

</xml_diff>

<commit_message>
color and format fig updates
</commit_message>
<xml_diff>
--- a/Functions and Code/Color Palette.xlsx
+++ b/Functions and Code/Color Palette.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evynd\Documents\matlabroot\Functions and Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yaleedu-my.sharepoint.com/personal/rebecca_ray_yale_edu/Documents/Documents/GitHub/matlabroot/Functions and Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D16787-DB1E-4B30-B3D4-75BF82E15E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{C5D16787-DB1E-4B30-B3D4-75BF82E15E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCDCE32B-C783-49D0-AFF8-1D1FC98F0417}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="33390" windowHeight="20985" xr2:uid="{B90EF345-F11D-4BE8-9704-8686C964E4D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B90EF345-F11D-4BE8-9704-8686C964E4D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="544">
   <si>
     <t>GreenYellow</t>
   </si>
@@ -1655,6 +1655,9 @@
   </si>
   <si>
     <t>186.225.255</t>
+  </si>
+  <si>
+    <t>Grey</t>
   </si>
 </sst>
 </file>
@@ -3006,7 +3009,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="242">
+  <cellXfs count="241">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3656,7 +3659,6 @@
     <xf numFmtId="0" fontId="0" fillId="164" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="165" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3744,9 +3746,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3784,7 +3786,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3890,7 +3892,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4032,7 +4034,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4040,10 +4042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBF5F8C-DD5F-4ED3-9E54-88EB7CF98784}">
-  <dimension ref="A1:E194"/>
+  <dimension ref="A1:D194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F194" sqref="F194"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G149" sqref="G149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5774,7 +5776,7 @@
     </row>
     <row r="147" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="24" t="s">
-        <v>297</v>
+        <v>543</v>
       </c>
       <c r="B147" s="24">
         <v>808080</v>
@@ -5936,7 +5938,7 @@
       </c>
       <c r="D160" s="208"/>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="24" t="s">
         <v>449</v>
       </c>
@@ -5948,7 +5950,7 @@
       </c>
       <c r="D161" s="209"/>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="24" t="s">
         <v>450</v>
       </c>
@@ -5960,7 +5962,7 @@
       </c>
       <c r="D162" s="210"/>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="24" t="s">
         <v>451</v>
       </c>
@@ -5972,7 +5974,7 @@
       </c>
       <c r="D163" s="211"/>
     </row>
-    <row r="164" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="199" t="s">
         <v>506</v>
       </c>
@@ -5980,7 +5982,7 @@
       <c r="C164" s="199"/>
       <c r="D164" s="199"/>
     </row>
-    <row r="165" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="24" t="s">
         <v>520</v>
       </c>
@@ -5990,9 +5992,9 @@
       <c r="C165" s="170" t="s">
         <v>512</v>
       </c>
-      <c r="D165" s="235"/>
-    </row>
-    <row r="166" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D165" s="234"/>
+    </row>
+    <row r="166" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="24" t="s">
         <v>521</v>
       </c>
@@ -6002,9 +6004,9 @@
       <c r="C166" s="170" t="s">
         <v>513</v>
       </c>
-      <c r="D166" s="231"/>
-    </row>
-    <row r="167" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D166" s="230"/>
+    </row>
+    <row r="167" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="24" t="s">
         <v>519</v>
       </c>
@@ -6014,9 +6016,9 @@
       <c r="C167" s="170" t="s">
         <v>514</v>
       </c>
-      <c r="D167" s="232"/>
-    </row>
-    <row r="168" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D167" s="231"/>
+    </row>
+    <row r="168" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="24" t="s">
         <v>517</v>
       </c>
@@ -6026,9 +6028,9 @@
       <c r="C168" s="170" t="s">
         <v>515</v>
       </c>
-      <c r="D168" s="233"/>
-    </row>
-    <row r="169" spans="1:5" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="D168" s="232"/>
+    </row>
+    <row r="169" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A169" s="24" t="s">
         <v>518</v>
       </c>
@@ -6038,9 +6040,9 @@
       <c r="C169" s="170" t="s">
         <v>516</v>
       </c>
-      <c r="D169" s="234"/>
-    </row>
-    <row r="170" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D169" s="233"/>
+    </row>
+    <row r="170" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="199" t="s">
         <v>458</v>
       </c>
@@ -6048,7 +6050,7 @@
       <c r="C170" s="199"/>
       <c r="D170" s="199"/>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="24" t="s">
         <v>472</v>
       </c>
@@ -6059,9 +6061,8 @@
         <v>461</v>
       </c>
       <c r="D171" s="215"/>
-      <c r="E171" s="221"/>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="24" t="s">
         <v>471</v>
       </c>
@@ -6073,7 +6074,7 @@
       </c>
       <c r="D172" s="217"/>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="24" t="s">
         <v>470</v>
       </c>
@@ -6085,7 +6086,7 @@
       </c>
       <c r="D173" s="218"/>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="24" t="s">
         <v>469</v>
       </c>
@@ -6097,7 +6098,7 @@
       </c>
       <c r="D174" s="219"/>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="24" t="s">
         <v>473</v>
       </c>
@@ -6109,7 +6110,7 @@
       </c>
       <c r="D175" s="220"/>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="24" t="s">
         <v>476</v>
       </c>
@@ -6139,7 +6140,7 @@
       <c r="C178" s="170" t="s">
         <v>483</v>
       </c>
-      <c r="D178" s="222"/>
+      <c r="D178" s="221"/>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="24" t="s">
@@ -6151,7 +6152,7 @@
       <c r="C179" s="24" t="s">
         <v>484</v>
       </c>
-      <c r="D179" s="223"/>
+      <c r="D179" s="222"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="24" t="s">
@@ -6163,7 +6164,7 @@
       <c r="C180" s="24" t="s">
         <v>485</v>
       </c>
-      <c r="D180" s="224"/>
+      <c r="D180" s="223"/>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="24" t="s">
@@ -6175,7 +6176,7 @@
       <c r="C181" s="24" t="s">
         <v>486</v>
       </c>
-      <c r="D181" s="225"/>
+      <c r="D181" s="224"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="24" t="s">
@@ -6187,7 +6188,7 @@
       <c r="C182" s="24" t="s">
         <v>487</v>
       </c>
-      <c r="D182" s="226"/>
+      <c r="D182" s="225"/>
     </row>
     <row r="183" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="199" t="s">
@@ -6207,7 +6208,7 @@
       <c r="C184" s="170" t="s">
         <v>498</v>
       </c>
-      <c r="D184" s="227"/>
+      <c r="D184" s="226"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="24" t="s">
@@ -6219,7 +6220,7 @@
       <c r="C185" s="24" t="s">
         <v>499</v>
       </c>
-      <c r="D185" s="228"/>
+      <c r="D185" s="227"/>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="24" t="s">
@@ -6231,7 +6232,7 @@
       <c r="C186" s="24" t="s">
         <v>500</v>
       </c>
-      <c r="D186" s="229"/>
+      <c r="D186" s="228"/>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="24" t="s">
@@ -6243,7 +6244,7 @@
       <c r="C187" s="24" t="s">
         <v>501</v>
       </c>
-      <c r="D187" s="230"/>
+      <c r="D187" s="229"/>
     </row>
     <row r="188" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="199" t="s">
@@ -6263,7 +6264,7 @@
       <c r="C189" s="170" t="s">
         <v>530</v>
       </c>
-      <c r="D189" s="240"/>
+      <c r="D189" s="239"/>
     </row>
     <row r="190" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="24" t="s">
@@ -6275,7 +6276,7 @@
       <c r="C190" s="170" t="s">
         <v>531</v>
       </c>
-      <c r="D190" s="236"/>
+      <c r="D190" s="235"/>
     </row>
     <row r="191" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="24" t="s">
@@ -6287,7 +6288,7 @@
       <c r="C191" s="170" t="s">
         <v>532</v>
       </c>
-      <c r="D191" s="237"/>
+      <c r="D191" s="236"/>
     </row>
     <row r="192" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="24" t="s">
@@ -6299,7 +6300,7 @@
       <c r="C192" s="170" t="s">
         <v>533</v>
       </c>
-      <c r="D192" s="238"/>
+      <c r="D192" s="237"/>
     </row>
     <row r="193" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A193" s="24" t="s">
@@ -6311,7 +6312,7 @@
       <c r="C193" s="170" t="s">
         <v>534</v>
       </c>
-      <c r="D193" s="239"/>
+      <c r="D193" s="238"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="24" t="s">
@@ -6323,7 +6324,7 @@
       <c r="C194" s="170" t="s">
         <v>529</v>
       </c>
-      <c r="D194" s="241"/>
+      <c r="D194" s="240"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
data blitz code updates
</commit_message>
<xml_diff>
--- a/Functions and Code/Color Palette.xlsx
+++ b/Functions and Code/Color Palette.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evynd\Documents\matlabroot\Functions and Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evyndickinson/Documents/matlabroot/Functions and Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF3EB2D-46CE-4DD2-BB4F-89D61CCAB638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6EC13C-3921-7244-9FEF-4BB8A6C03E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="33390" windowHeight="20985" xr2:uid="{B90EF345-F11D-4BE8-9704-8686C964E4D8}"/>
+    <workbookView xWindow="0" yWindow="580" windowWidth="29920" windowHeight="18760" xr2:uid="{B90EF345-F11D-4BE8-9704-8686C964E4D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3746,9 +3746,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3786,7 +3786,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3892,7 +3892,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4034,7 +4034,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4044,25 +4044,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBF5F8C-DD5F-4ED3-9E54-88EB7CF98784}">
   <dimension ref="A1:D195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E147" sqref="E147"/>
+    <sheetView tabSelected="1" topLeftCell="A155" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E168" sqref="E168"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="170" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" style="24" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" customWidth="1"/>
-    <col min="20" max="20" width="19.85546875" customWidth="1"/>
-    <col min="23" max="23" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="170" customWidth="1"/>
+    <col min="4" max="4" width="6.5" style="24" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.6640625" customWidth="1"/>
+    <col min="20" max="20" width="19.83203125" customWidth="1"/>
+    <col min="23" max="23" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="162" t="s">
         <v>305</v>
       </c>
@@ -4070,7 +4070,7 @@
       <c r="C1" s="169"/>
       <c r="D1" s="164"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>54</v>
       </c>
@@ -4082,7 +4082,7 @@
       </c>
       <c r="D2" s="48"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>56</v>
       </c>
@@ -4094,7 +4094,7 @@
       </c>
       <c r="D3" s="49"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>58</v>
       </c>
@@ -4106,7 +4106,7 @@
       </c>
       <c r="D4" s="50"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>60</v>
       </c>
@@ -4118,7 +4118,7 @@
       </c>
       <c r="D5" s="51"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>62</v>
       </c>
@@ -4130,7 +4130,7 @@
       </c>
       <c r="D6" s="52"/>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>64</v>
       </c>
@@ -4142,7 +4142,7 @@
       </c>
       <c r="D7" s="53"/>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>66</v>
       </c>
@@ -4154,7 +4154,7 @@
       </c>
       <c r="D8" s="54"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>68</v>
       </c>
@@ -4166,7 +4166,7 @@
       </c>
       <c r="D9" s="55"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
         <v>70</v>
       </c>
@@ -4178,7 +4178,7 @@
       </c>
       <c r="D10" s="152"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="159" t="s">
         <v>72</v>
       </c>
@@ -4186,7 +4186,7 @@
       <c r="C11" s="171"/>
       <c r="D11" s="161"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
         <v>73</v>
       </c>
@@ -4198,7 +4198,7 @@
       </c>
       <c r="D12" s="56"/>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>75</v>
       </c>
@@ -4210,7 +4210,7 @@
       </c>
       <c r="D13" s="57"/>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>77</v>
       </c>
@@ -4222,7 +4222,7 @@
       </c>
       <c r="D14" s="58"/>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>79</v>
       </c>
@@ -4234,7 +4234,7 @@
       </c>
       <c r="D15" s="59"/>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>81</v>
       </c>
@@ -4246,7 +4246,7 @@
       </c>
       <c r="D16" s="60"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>83</v>
       </c>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="D17" s="165"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="167" t="s">
         <v>85</v>
       </c>
@@ -4266,7 +4266,7 @@
       <c r="C18" s="172"/>
       <c r="D18" s="166"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>86</v>
       </c>
@@ -4278,7 +4278,7 @@
       </c>
       <c r="D19" s="61"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>88</v>
       </c>
@@ -4290,7 +4290,7 @@
       </c>
       <c r="D20" s="62"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
         <v>90</v>
       </c>
@@ -4302,7 +4302,7 @@
       </c>
       <c r="D21" s="63"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
         <v>92</v>
       </c>
@@ -4314,7 +4314,7 @@
       </c>
       <c r="D22" s="64"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
         <v>94</v>
       </c>
@@ -4326,7 +4326,7 @@
       </c>
       <c r="D23" s="151"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="156" t="s">
         <v>96</v>
       </c>
@@ -4334,7 +4334,7 @@
       <c r="C24" s="173"/>
       <c r="D24" s="158"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
         <v>97</v>
       </c>
@@ -4346,7 +4346,7 @@
       </c>
       <c r="D25" s="65"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
         <v>99</v>
       </c>
@@ -4358,7 +4358,7 @@
       </c>
       <c r="D26" s="66"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
         <v>101</v>
       </c>
@@ -4370,7 +4370,7 @@
       </c>
       <c r="D27" s="67"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
         <v>103</v>
       </c>
@@ -4382,7 +4382,7 @@
       </c>
       <c r="D28" s="68"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
         <v>105</v>
       </c>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="D29" s="69"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
         <v>107</v>
       </c>
@@ -4406,7 +4406,7 @@
       </c>
       <c r="D30" s="70"/>
     </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
         <v>109</v>
       </c>
@@ -4418,7 +4418,7 @@
       </c>
       <c r="D31" s="71"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
         <v>111</v>
       </c>
@@ -4430,7 +4430,7 @@
       </c>
       <c r="D32" s="72"/>
     </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
         <v>113</v>
       </c>
@@ -4442,7 +4442,7 @@
       </c>
       <c r="D33" s="73"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
         <v>115</v>
       </c>
@@ -4454,7 +4454,7 @@
       </c>
       <c r="D34" s="74"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
         <v>117</v>
       </c>
@@ -4466,7 +4466,7 @@
       </c>
       <c r="D35" s="150"/>
     </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="153" t="s">
         <v>119</v>
       </c>
@@ -4474,7 +4474,7 @@
       <c r="C36" s="174"/>
       <c r="D36" s="155"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>120</v>
       </c>
@@ -4486,7 +4486,7 @@
       </c>
       <c r="D37" s="75"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
         <v>122</v>
       </c>
@@ -4498,7 +4498,7 @@
       </c>
       <c r="D38" s="76"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>124</v>
       </c>
@@ -4510,7 +4510,7 @@
       </c>
       <c r="D39" s="77"/>
     </row>
-    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>126</v>
       </c>
@@ -4522,7 +4522,7 @@
       </c>
       <c r="D40" s="78"/>
     </row>
-    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>128</v>
       </c>
@@ -4534,7 +4534,7 @@
       </c>
       <c r="D41" s="79"/>
     </row>
-    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>130</v>
       </c>
@@ -4546,7 +4546,7 @@
       </c>
       <c r="D42" s="80"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>132</v>
       </c>
@@ -4558,7 +4558,7 @@
       </c>
       <c r="D43" s="80"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="24" t="s">
         <v>133</v>
       </c>
@@ -4570,7 +4570,7 @@
       </c>
       <c r="D44" s="81"/>
     </row>
-    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="24" t="s">
         <v>135</v>
       </c>
@@ -4582,7 +4582,7 @@
       </c>
       <c r="D45" s="82"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="24" t="s">
         <v>137</v>
       </c>
@@ -4594,7 +4594,7 @@
       </c>
       <c r="D46" s="83"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
         <v>139</v>
       </c>
@@ -4606,7 +4606,7 @@
       </c>
       <c r="D47" s="84"/>
     </row>
-    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
         <v>141</v>
       </c>
@@ -4618,7 +4618,7 @@
       </c>
       <c r="D48" s="85"/>
     </row>
-    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
         <v>143</v>
       </c>
@@ -4630,7 +4630,7 @@
       </c>
       <c r="D49" s="86"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
         <v>145</v>
       </c>
@@ -4642,7 +4642,7 @@
       </c>
       <c r="D50" s="87"/>
     </row>
-    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
         <v>146</v>
       </c>
@@ -4654,7 +4654,7 @@
       </c>
       <c r="D51" s="88"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="24" t="s">
         <v>147</v>
       </c>
@@ -4666,7 +4666,7 @@
       </c>
       <c r="D52" s="89"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
         <v>149</v>
       </c>
@@ -4678,7 +4678,7 @@
       </c>
       <c r="D53" s="90"/>
     </row>
-    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
         <v>151</v>
       </c>
@@ -4690,7 +4690,7 @@
       </c>
       <c r="D54" s="91"/>
     </row>
-    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
         <v>153</v>
       </c>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="D55" s="92"/>
     </row>
-    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="147" t="s">
         <v>155</v>
       </c>
@@ -4710,7 +4710,7 @@
       <c r="C56" s="175"/>
       <c r="D56" s="149"/>
     </row>
-    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="24" t="s">
         <v>0</v>
       </c>
@@ -4722,7 +4722,7 @@
       </c>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="24" t="s">
         <v>2</v>
       </c>
@@ -4734,7 +4734,7 @@
       </c>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="24" t="s">
         <v>4</v>
       </c>
@@ -4746,7 +4746,7 @@
       </c>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="24" t="s">
         <v>6</v>
       </c>
@@ -4758,7 +4758,7 @@
       </c>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="24" t="s">
         <v>8</v>
       </c>
@@ -4770,7 +4770,7 @@
       </c>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="24" t="s">
         <v>10</v>
       </c>
@@ -4782,7 +4782,7 @@
       </c>
       <c r="D62" s="6"/>
     </row>
-    <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="24" t="s">
         <v>12</v>
       </c>
@@ -4794,7 +4794,7 @@
       </c>
       <c r="D63" s="7"/>
     </row>
-    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="24" t="s">
         <v>14</v>
       </c>
@@ -4806,7 +4806,7 @@
       </c>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="24" t="s">
         <v>17</v>
       </c>
@@ -4818,7 +4818,7 @@
       </c>
       <c r="D65" s="9"/>
     </row>
-    <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="24" t="s">
         <v>20</v>
       </c>
@@ -4830,7 +4830,7 @@
       </c>
       <c r="D66" s="10"/>
     </row>
-    <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="24" t="s">
         <v>22</v>
       </c>
@@ -4842,7 +4842,7 @@
       </c>
       <c r="D67" s="11"/>
     </row>
-    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="24" t="s">
         <v>25</v>
       </c>
@@ -4854,7 +4854,7 @@
       </c>
       <c r="D68" s="12"/>
     </row>
-    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="24" t="s">
         <v>28</v>
       </c>
@@ -4866,7 +4866,7 @@
       </c>
       <c r="D69" s="13"/>
     </row>
-    <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="24" t="s">
         <v>30</v>
       </c>
@@ -4878,7 +4878,7 @@
       </c>
       <c r="D70" s="14"/>
     </row>
-    <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="24" t="s">
         <v>32</v>
       </c>
@@ -4890,7 +4890,7 @@
       </c>
       <c r="D71" s="15"/>
     </row>
-    <row r="72" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="24" t="s">
         <v>35</v>
       </c>
@@ -4902,7 +4902,7 @@
       </c>
       <c r="D72" s="16"/>
     </row>
-    <row r="73" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="24" t="s">
         <v>38</v>
       </c>
@@ -4914,7 +4914,7 @@
       </c>
       <c r="D73" s="17"/>
     </row>
-    <row r="74" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="24" t="s">
         <v>40</v>
       </c>
@@ -4926,7 +4926,7 @@
       </c>
       <c r="D74" s="18"/>
     </row>
-    <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="24" t="s">
         <v>43</v>
       </c>
@@ -4938,7 +4938,7 @@
       </c>
       <c r="D75" s="19"/>
     </row>
-    <row r="76" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="24" t="s">
         <v>45</v>
       </c>
@@ -4950,7 +4950,7 @@
       </c>
       <c r="D76" s="20"/>
     </row>
-    <row r="77" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="24" t="s">
         <v>47</v>
       </c>
@@ -4962,7 +4962,7 @@
       </c>
       <c r="D77" s="21"/>
     </row>
-    <row r="78" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="24" t="s">
         <v>49</v>
       </c>
@@ -4974,7 +4974,7 @@
       </c>
       <c r="D78" s="22"/>
     </row>
-    <row r="79" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="24" t="s">
         <v>52</v>
       </c>
@@ -4986,7 +4986,7 @@
       </c>
       <c r="D79" s="23"/>
     </row>
-    <row r="80" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="144" t="s">
         <v>156</v>
       </c>
@@ -4994,7 +4994,7 @@
       <c r="C80" s="176"/>
       <c r="D80" s="146"/>
     </row>
-    <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="24" t="s">
         <v>157</v>
       </c>
@@ -5006,7 +5006,7 @@
       </c>
       <c r="D81" s="25"/>
     </row>
-    <row r="82" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="24" t="s">
         <v>160</v>
       </c>
@@ -5018,7 +5018,7 @@
       </c>
       <c r="D82" s="25"/>
     </row>
-    <row r="83" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="24" t="s">
         <v>161</v>
       </c>
@@ -5030,7 +5030,7 @@
       </c>
       <c r="D83" s="26"/>
     </row>
-    <row r="84" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="24" t="s">
         <v>163</v>
       </c>
@@ -5042,7 +5042,7 @@
       </c>
       <c r="D84" s="27"/>
     </row>
-    <row r="85" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="24" t="s">
         <v>165</v>
       </c>
@@ -5054,7 +5054,7 @@
       </c>
       <c r="D85" s="28"/>
     </row>
-    <row r="86" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="24" t="s">
         <v>167</v>
       </c>
@@ -5066,7 +5066,7 @@
       </c>
       <c r="D86" s="29"/>
     </row>
-    <row r="87" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="24" t="s">
         <v>169</v>
       </c>
@@ -5078,7 +5078,7 @@
       </c>
       <c r="D87" s="30"/>
     </row>
-    <row r="88" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="24" t="s">
         <v>171</v>
       </c>
@@ -5090,7 +5090,7 @@
       </c>
       <c r="D88" s="31"/>
     </row>
-    <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="24" t="s">
         <v>174</v>
       </c>
@@ -5102,7 +5102,7 @@
       </c>
       <c r="D89" s="32"/>
     </row>
-    <row r="90" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="24" t="s">
         <v>176</v>
       </c>
@@ -5114,7 +5114,7 @@
       </c>
       <c r="D90" s="33"/>
     </row>
-    <row r="91" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" s="24" t="s">
         <v>178</v>
       </c>
@@ -5126,7 +5126,7 @@
       </c>
       <c r="D91" s="34"/>
     </row>
-    <row r="92" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="24" t="s">
         <v>180</v>
       </c>
@@ -5138,7 +5138,7 @@
       </c>
       <c r="D92" s="35"/>
     </row>
-    <row r="93" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" s="24" t="s">
         <v>182</v>
       </c>
@@ -5150,7 +5150,7 @@
       </c>
       <c r="D93" s="36"/>
     </row>
-    <row r="94" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="24" t="s">
         <v>184</v>
       </c>
@@ -5162,7 +5162,7 @@
       </c>
       <c r="D94" s="37"/>
     </row>
-    <row r="95" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A95" s="24" t="s">
         <v>186</v>
       </c>
@@ -5174,7 +5174,7 @@
       </c>
       <c r="D95" s="38"/>
     </row>
-    <row r="96" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A96" s="24" t="s">
         <v>188</v>
       </c>
@@ -5186,7 +5186,7 @@
       </c>
       <c r="D96" s="39"/>
     </row>
-    <row r="97" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="24" t="s">
         <v>191</v>
       </c>
@@ -5198,7 +5198,7 @@
       </c>
       <c r="D97" s="40"/>
     </row>
-    <row r="98" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="24" t="s">
         <v>193</v>
       </c>
@@ -5210,7 +5210,7 @@
       </c>
       <c r="D98" s="41"/>
     </row>
-    <row r="99" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="24" t="s">
         <v>195</v>
       </c>
@@ -5222,7 +5222,7 @@
       </c>
       <c r="D99" s="42"/>
     </row>
-    <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A100" s="24" t="s">
         <v>196</v>
       </c>
@@ -5234,7 +5234,7 @@
       </c>
       <c r="D100" s="43"/>
     </row>
-    <row r="101" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="24" t="s">
         <v>199</v>
       </c>
@@ -5246,7 +5246,7 @@
       </c>
       <c r="D101" s="44"/>
     </row>
-    <row r="102" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A102" s="24" t="s">
         <v>202</v>
       </c>
@@ -5258,7 +5258,7 @@
       </c>
       <c r="D102" s="45"/>
     </row>
-    <row r="103" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="24" t="s">
         <v>205</v>
       </c>
@@ -5270,7 +5270,7 @@
       </c>
       <c r="D103" s="46"/>
     </row>
-    <row r="104" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="24" t="s">
         <v>207</v>
       </c>
@@ -5282,7 +5282,7 @@
       </c>
       <c r="D104" s="47"/>
     </row>
-    <row r="105" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="141" t="s">
         <v>209</v>
       </c>
@@ -5290,7 +5290,7 @@
       <c r="C105" s="177"/>
       <c r="D105" s="143"/>
     </row>
-    <row r="106" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" s="24" t="s">
         <v>210</v>
       </c>
@@ -5302,7 +5302,7 @@
       </c>
       <c r="D106" s="93"/>
     </row>
-    <row r="107" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A107" s="24" t="s">
         <v>212</v>
       </c>
@@ -5314,7 +5314,7 @@
       </c>
       <c r="D107" s="94"/>
     </row>
-    <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A108" s="24" t="s">
         <v>214</v>
       </c>
@@ -5326,7 +5326,7 @@
       </c>
       <c r="D108" s="95"/>
     </row>
-    <row r="109" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A109" s="24" t="s">
         <v>216</v>
       </c>
@@ -5338,7 +5338,7 @@
       </c>
       <c r="D109" s="96"/>
     </row>
-    <row r="110" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A110" s="24" t="s">
         <v>218</v>
       </c>
@@ -5350,7 +5350,7 @@
       </c>
       <c r="D110" s="97"/>
     </row>
-    <row r="111" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A111" s="24" t="s">
         <v>220</v>
       </c>
@@ -5362,7 +5362,7 @@
       </c>
       <c r="D111" s="98"/>
     </row>
-    <row r="112" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A112" s="24" t="s">
         <v>222</v>
       </c>
@@ -5374,7 +5374,7 @@
       </c>
       <c r="D112" s="99"/>
     </row>
-    <row r="113" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A113" s="24" t="s">
         <v>224</v>
       </c>
@@ -5386,7 +5386,7 @@
       </c>
       <c r="D113" s="100"/>
     </row>
-    <row r="114" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A114" s="24" t="s">
         <v>226</v>
       </c>
@@ -5398,7 +5398,7 @@
       </c>
       <c r="D114" s="101"/>
     </row>
-    <row r="115" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A115" s="24" t="s">
         <v>229</v>
       </c>
@@ -5410,7 +5410,7 @@
       </c>
       <c r="D115" s="102"/>
     </row>
-    <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A116" s="24" t="s">
         <v>232</v>
       </c>
@@ -5422,7 +5422,7 @@
       </c>
       <c r="D116" s="103"/>
     </row>
-    <row r="117" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A117" s="24" t="s">
         <v>235</v>
       </c>
@@ -5434,7 +5434,7 @@
       </c>
       <c r="D117" s="104"/>
     </row>
-    <row r="118" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="24" t="s">
         <v>238</v>
       </c>
@@ -5446,7 +5446,7 @@
       </c>
       <c r="D118" s="105"/>
     </row>
-    <row r="119" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A119" s="24" t="s">
         <v>241</v>
       </c>
@@ -5458,7 +5458,7 @@
       </c>
       <c r="D119" s="106"/>
     </row>
-    <row r="120" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A120" s="24" t="s">
         <v>244</v>
       </c>
@@ -5470,7 +5470,7 @@
       </c>
       <c r="D120" s="107"/>
     </row>
-    <row r="121" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A121" s="24" t="s">
         <v>247</v>
       </c>
@@ -5482,7 +5482,7 @@
       </c>
       <c r="D121" s="108"/>
     </row>
-    <row r="122" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A122" s="24" t="s">
         <v>250</v>
       </c>
@@ -5494,7 +5494,7 @@
       </c>
       <c r="D122" s="132"/>
     </row>
-    <row r="123" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A123" s="135" t="s">
         <v>252</v>
       </c>
@@ -5502,7 +5502,7 @@
       <c r="C123" s="178"/>
       <c r="D123" s="134"/>
     </row>
-    <row r="124" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A124" s="24" t="s">
         <v>253</v>
       </c>
@@ -5514,7 +5514,7 @@
       </c>
       <c r="D124" s="88"/>
     </row>
-    <row r="125" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A125" s="24" t="s">
         <v>255</v>
       </c>
@@ -5526,7 +5526,7 @@
       </c>
       <c r="D125" s="109"/>
     </row>
-    <row r="126" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A126" s="24" t="s">
         <v>257</v>
       </c>
@@ -5538,7 +5538,7 @@
       </c>
       <c r="D126" s="110"/>
     </row>
-    <row r="127" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A127" s="24" t="s">
         <v>259</v>
       </c>
@@ -5550,7 +5550,7 @@
       </c>
       <c r="D127" s="111"/>
     </row>
-    <row r="128" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A128" s="24" t="s">
         <v>261</v>
       </c>
@@ -5562,7 +5562,7 @@
       </c>
       <c r="D128" s="112"/>
     </row>
-    <row r="129" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A129" s="24" t="s">
         <v>263</v>
       </c>
@@ -5574,7 +5574,7 @@
       </c>
       <c r="D129" s="113"/>
     </row>
-    <row r="130" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A130" s="24" t="s">
         <v>265</v>
       </c>
@@ -5586,7 +5586,7 @@
       </c>
       <c r="D130" s="114"/>
     </row>
-    <row r="131" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A131" s="24" t="s">
         <v>267</v>
       </c>
@@ -5598,7 +5598,7 @@
       </c>
       <c r="D131" s="115"/>
     </row>
-    <row r="132" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A132" s="24" t="s">
         <v>269</v>
       </c>
@@ -5610,7 +5610,7 @@
       </c>
       <c r="D132" s="116"/>
     </row>
-    <row r="133" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A133" s="24" t="s">
         <v>271</v>
       </c>
@@ -5622,7 +5622,7 @@
       </c>
       <c r="D133" s="117"/>
     </row>
-    <row r="134" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A134" s="24" t="s">
         <v>273</v>
       </c>
@@ -5634,7 +5634,7 @@
       </c>
       <c r="D134" s="118"/>
     </row>
-    <row r="135" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A135" s="24" t="s">
         <v>275</v>
       </c>
@@ -5646,7 +5646,7 @@
       </c>
       <c r="D135" s="119"/>
     </row>
-    <row r="136" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A136" s="24" t="s">
         <v>277</v>
       </c>
@@ -5658,7 +5658,7 @@
       </c>
       <c r="D136" s="120"/>
     </row>
-    <row r="137" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A137" s="24" t="s">
         <v>279</v>
       </c>
@@ -5670,7 +5670,7 @@
       </c>
       <c r="D137" s="121"/>
     </row>
-    <row r="138" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A138" s="24" t="s">
         <v>281</v>
       </c>
@@ -5682,7 +5682,7 @@
       </c>
       <c r="D138" s="122"/>
     </row>
-    <row r="139" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A139" s="24" t="s">
         <v>283</v>
       </c>
@@ -5694,7 +5694,7 @@
       </c>
       <c r="D139" s="123"/>
     </row>
-    <row r="140" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A140" s="24" t="s">
         <v>285</v>
       </c>
@@ -5706,7 +5706,7 @@
       </c>
       <c r="D140" s="136"/>
     </row>
-    <row r="141" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A141" s="138" t="s">
         <v>287</v>
       </c>
@@ -5714,7 +5714,7 @@
       <c r="C141" s="179"/>
       <c r="D141" s="140"/>
     </row>
-    <row r="142" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A142" s="24" t="s">
         <v>288</v>
       </c>
@@ -5726,7 +5726,7 @@
       </c>
       <c r="D142" s="124"/>
     </row>
-    <row r="143" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A143" s="24" t="s">
         <v>290</v>
       </c>
@@ -5738,7 +5738,7 @@
       </c>
       <c r="D143" s="125"/>
     </row>
-    <row r="144" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A144" s="24" t="s">
         <v>292</v>
       </c>
@@ -5750,7 +5750,7 @@
       </c>
       <c r="D144" s="125"/>
     </row>
-    <row r="145" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A145" s="24" t="s">
         <v>293</v>
       </c>
@@ -5762,7 +5762,7 @@
       </c>
       <c r="D145" s="126"/>
     </row>
-    <row r="146" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A146" s="24" t="s">
         <v>295</v>
       </c>
@@ -5774,7 +5774,7 @@
       </c>
       <c r="D146" s="127"/>
     </row>
-    <row r="147" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A147" s="24" t="s">
         <v>543</v>
       </c>
@@ -5786,7 +5786,7 @@
       </c>
       <c r="D147" s="128"/>
     </row>
-    <row r="148" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A148" s="24" t="s">
         <v>297</v>
       </c>
@@ -5798,7 +5798,7 @@
       </c>
       <c r="D148" s="128"/>
     </row>
-    <row r="149" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A149" s="24" t="s">
         <v>298</v>
       </c>
@@ -5810,7 +5810,7 @@
       </c>
       <c r="D149" s="129"/>
     </row>
-    <row r="150" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A150" s="24" t="s">
         <v>299</v>
       </c>
@@ -5822,7 +5822,7 @@
       </c>
       <c r="D150" s="130"/>
     </row>
-    <row r="151" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A151" s="24" t="s">
         <v>300</v>
       </c>
@@ -5834,7 +5834,7 @@
       </c>
       <c r="D151" s="131"/>
     </row>
-    <row r="152" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A152" s="24" t="s">
         <v>301</v>
       </c>
@@ -5846,7 +5846,7 @@
       </c>
       <c r="D152" s="197"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="24" t="s">
         <v>303</v>
       </c>
@@ -5858,7 +5858,7 @@
       </c>
       <c r="D153" s="198"/>
     </row>
-    <row r="154" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A154" s="199" t="s">
         <v>443</v>
       </c>
@@ -5866,7 +5866,7 @@
       <c r="C154" s="200"/>
       <c r="D154" s="199"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="24" t="s">
         <v>427</v>
       </c>
@@ -5878,7 +5878,7 @@
       </c>
       <c r="D155" s="201"/>
     </row>
-    <row r="156" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A156" s="24" t="s">
         <v>436</v>
       </c>
@@ -5890,7 +5890,7 @@
       </c>
       <c r="D156" s="205"/>
     </row>
-    <row r="157" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A157" s="24" t="s">
         <v>437</v>
       </c>
@@ -5902,7 +5902,7 @@
       </c>
       <c r="D157" s="202"/>
     </row>
-    <row r="158" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A158" s="24" t="s">
         <v>438</v>
       </c>
@@ -5914,7 +5914,7 @@
       </c>
       <c r="D158" s="203"/>
     </row>
-    <row r="159" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" ht="21" x14ac:dyDescent="0.2">
       <c r="A159" s="24" t="s">
         <v>439</v>
       </c>
@@ -5926,7 +5926,7 @@
       </c>
       <c r="D159" s="204"/>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="24" t="s">
         <v>442</v>
       </c>
@@ -5938,7 +5938,7 @@
       </c>
       <c r="D160" s="206"/>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="24" t="s">
         <v>448</v>
       </c>
@@ -5950,7 +5950,7 @@
       </c>
       <c r="D161" s="208"/>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="24" t="s">
         <v>449</v>
       </c>
@@ -5962,7 +5962,7 @@
       </c>
       <c r="D162" s="209"/>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="24" t="s">
         <v>450</v>
       </c>
@@ -5974,7 +5974,7 @@
       </c>
       <c r="D163" s="210"/>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="24" t="s">
         <v>451</v>
       </c>
@@ -5986,7 +5986,7 @@
       </c>
       <c r="D164" s="211"/>
     </row>
-    <row r="165" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A165" s="199" t="s">
         <v>506</v>
       </c>
@@ -5994,7 +5994,7 @@
       <c r="C165" s="199"/>
       <c r="D165" s="199"/>
     </row>
-    <row r="166" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A166" s="24" t="s">
         <v>520</v>
       </c>
@@ -6006,7 +6006,7 @@
       </c>
       <c r="D166" s="234"/>
     </row>
-    <row r="167" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A167" s="24" t="s">
         <v>521</v>
       </c>
@@ -6018,7 +6018,7 @@
       </c>
       <c r="D167" s="230"/>
     </row>
-    <row r="168" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A168" s="24" t="s">
         <v>519</v>
       </c>
@@ -6030,7 +6030,7 @@
       </c>
       <c r="D168" s="231"/>
     </row>
-    <row r="169" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A169" s="24" t="s">
         <v>517</v>
       </c>
@@ -6042,7 +6042,7 @@
       </c>
       <c r="D169" s="232"/>
     </row>
-    <row r="170" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" ht="21" x14ac:dyDescent="0.2">
       <c r="A170" s="24" t="s">
         <v>518</v>
       </c>
@@ -6054,7 +6054,7 @@
       </c>
       <c r="D170" s="233"/>
     </row>
-    <row r="171" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A171" s="199" t="s">
         <v>458</v>
       </c>
@@ -6062,7 +6062,7 @@
       <c r="C171" s="199"/>
       <c r="D171" s="199"/>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="24" t="s">
         <v>472</v>
       </c>
@@ -6074,7 +6074,7 @@
       </c>
       <c r="D172" s="215"/>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="24" t="s">
         <v>471</v>
       </c>
@@ -6086,7 +6086,7 @@
       </c>
       <c r="D173" s="217"/>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="24" t="s">
         <v>470</v>
       </c>
@@ -6098,7 +6098,7 @@
       </c>
       <c r="D174" s="218"/>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" s="24" t="s">
         <v>469</v>
       </c>
@@ -6110,7 +6110,7 @@
       </c>
       <c r="D175" s="219"/>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="24" t="s">
         <v>473</v>
       </c>
@@ -6122,7 +6122,7 @@
       </c>
       <c r="D176" s="220"/>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" s="24" t="s">
         <v>476</v>
       </c>
@@ -6134,7 +6134,7 @@
       </c>
       <c r="D177" s="216"/>
     </row>
-    <row r="178" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A178" s="199" t="s">
         <v>477</v>
       </c>
@@ -6142,7 +6142,7 @@
       <c r="C178" s="199"/>
       <c r="D178" s="199"/>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" s="24" t="s">
         <v>488</v>
       </c>
@@ -6154,7 +6154,7 @@
       </c>
       <c r="D179" s="221"/>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" s="24" t="s">
         <v>489</v>
       </c>
@@ -6166,7 +6166,7 @@
       </c>
       <c r="D180" s="222"/>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" s="24" t="s">
         <v>490</v>
       </c>
@@ -6178,7 +6178,7 @@
       </c>
       <c r="D181" s="223"/>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" s="24" t="s">
         <v>491</v>
       </c>
@@ -6190,7 +6190,7 @@
       </c>
       <c r="D182" s="224"/>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" s="24" t="s">
         <v>492</v>
       </c>
@@ -6202,7 +6202,7 @@
       </c>
       <c r="D183" s="225"/>
     </row>
-    <row r="184" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A184" s="199" t="s">
         <v>493</v>
       </c>
@@ -6210,7 +6210,7 @@
       <c r="C184" s="199"/>
       <c r="D184" s="199"/>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="24" t="s">
         <v>502</v>
       </c>
@@ -6222,7 +6222,7 @@
       </c>
       <c r="D185" s="226"/>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" s="24" t="s">
         <v>503</v>
       </c>
@@ -6234,7 +6234,7 @@
       </c>
       <c r="D186" s="227"/>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" s="24" t="s">
         <v>504</v>
       </c>
@@ -6246,7 +6246,7 @@
       </c>
       <c r="D187" s="228"/>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" s="24" t="s">
         <v>505</v>
       </c>
@@ -6258,7 +6258,7 @@
       </c>
       <c r="D188" s="229"/>
     </row>
-    <row r="189" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A189" s="199" t="s">
         <v>526</v>
       </c>
@@ -6266,7 +6266,7 @@
       <c r="C189" s="199"/>
       <c r="D189" s="199"/>
     </row>
-    <row r="190" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A190" s="24" t="s">
         <v>535</v>
       </c>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="D190" s="239"/>
     </row>
-    <row r="191" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A191" s="24" t="s">
         <v>536</v>
       </c>
@@ -6290,7 +6290,7 @@
       </c>
       <c r="D191" s="235"/>
     </row>
-    <row r="192" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A192" s="24" t="s">
         <v>537</v>
       </c>
@@ -6302,7 +6302,7 @@
       </c>
       <c r="D192" s="236"/>
     </row>
-    <row r="193" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A193" s="24" t="s">
         <v>538</v>
       </c>
@@ -6314,7 +6314,7 @@
       </c>
       <c r="D193" s="237"/>
     </row>
-    <row r="194" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" ht="21" x14ac:dyDescent="0.2">
       <c r="A194" s="24" t="s">
         <v>539</v>
       </c>
@@ -6326,7 +6326,7 @@
       </c>
       <c r="D194" s="238"/>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="24" t="s">
         <v>540</v>
       </c>
@@ -6352,21 +6352,17 @@
       <selection activeCell="I95" sqref="I95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.85546875"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="8.85546875"/>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" customWidth="1"/>
-    <col min="13" max="14" width="8.85546875"/>
-    <col min="15" max="15" width="19.85546875" customWidth="1"/>
-    <col min="16" max="17" width="8.85546875"/>
-    <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="15" max="15" width="19.83203125" customWidth="1"/>
+    <col min="18" max="18" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C1" s="212" t="s">
         <v>456</v>
       </c>
@@ -6377,7 +6373,7 @@
       <c r="F1" s="213"/>
       <c r="G1" s="214"/>
     </row>
-    <row r="6" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>414</v>
       </c>
@@ -6412,7 +6408,7 @@
       </c>
       <c r="O6" s="6"/>
     </row>
-    <row r="7" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>415</v>
       </c>
@@ -6447,7 +6443,7 @@
       </c>
       <c r="O7" s="10"/>
     </row>
-    <row r="8" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>416</v>
       </c>
@@ -6482,31 +6478,31 @@
       </c>
       <c r="O8" s="14"/>
     </row>
-    <row r="10" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:27" x14ac:dyDescent="0.2">
       <c r="W10" s="196"/>
       <c r="X10" s="196"/>
       <c r="Y10" s="196"/>
       <c r="Z10" s="196"/>
     </row>
-    <row r="11" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:27" x14ac:dyDescent="0.2">
       <c r="W11" s="196"/>
       <c r="X11" s="196"/>
       <c r="Y11" s="196"/>
       <c r="Z11" s="196"/>
     </row>
-    <row r="12" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:27" x14ac:dyDescent="0.2">
       <c r="W12" s="196"/>
       <c r="X12" s="196"/>
       <c r="Y12" s="196"/>
       <c r="Z12" s="196"/>
     </row>
-    <row r="13" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:27" x14ac:dyDescent="0.2">
       <c r="W13" s="196"/>
       <c r="X13" s="196"/>
       <c r="Y13" s="196"/>
       <c r="Z13" s="196"/>
     </row>
-    <row r="14" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C14" s="24" t="s">
         <v>79</v>
       </c>
@@ -6528,7 +6524,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="15" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C15" s="24" t="s">
         <v>94</v>
       </c>
@@ -6550,7 +6546,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="16" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C16" s="24" t="s">
         <v>6</v>
       </c>
@@ -6572,7 +6568,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C17" s="24" t="s">
         <v>191</v>
       </c>
@@ -6604,7 +6600,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H18" s="24" t="s">
         <v>160</v>
       </c>
@@ -6628,7 +6624,7 @@
       <c r="Y18" s="196"/>
       <c r="Z18" s="196"/>
     </row>
-    <row r="19" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H19" s="24" t="s">
         <v>191</v>
       </c>
@@ -6652,7 +6648,7 @@
       <c r="Y19" s="196"/>
       <c r="Z19" s="196"/>
     </row>
-    <row r="20" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H20" s="24" t="s">
         <v>202</v>
       </c>
@@ -6676,7 +6672,7 @@
       <c r="Y20" s="196"/>
       <c r="Z20" s="196"/>
     </row>
-    <row r="21" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C21" s="24" t="s">
         <v>75</v>
       </c>
@@ -6699,7 +6695,7 @@
       <c r="Y21" s="196"/>
       <c r="Z21" s="196"/>
     </row>
-    <row r="22" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C22" s="24" t="s">
         <v>79</v>
       </c>
@@ -6715,7 +6711,7 @@
       <c r="Y22" s="196"/>
       <c r="Z22" s="196"/>
     </row>
-    <row r="23" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C23" s="24" t="s">
         <v>191</v>
       </c>
@@ -6730,7 +6726,7 @@
       <c r="I23" s="24"/>
       <c r="J23" s="170"/>
     </row>
-    <row r="24" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C24" s="24" t="s">
         <v>186</v>
       </c>
@@ -6745,41 +6741,41 @@
       <c r="I24" s="24"/>
       <c r="J24" s="170"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="H25" s="24"/>
       <c r="I25" s="24"/>
       <c r="J25" s="170"/>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="H26" s="24"/>
       <c r="I26" s="24"/>
       <c r="J26" s="170"/>
     </row>
-    <row r="27" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C27" s="24" t="s">
         <v>88</v>
       </c>
       <c r="D27" s="62"/>
     </row>
-    <row r="28" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C28" s="24" t="s">
         <v>111</v>
       </c>
       <c r="D28" s="72"/>
     </row>
-    <row r="29" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C29" s="24" t="s">
         <v>180</v>
       </c>
       <c r="D29" s="35"/>
     </row>
-    <row r="30" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C30" s="24" t="s">
         <v>191</v>
       </c>
       <c r="D30" s="40"/>
     </row>
-    <row r="32" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
         <v>120</v>
       </c>
@@ -6798,7 +6794,7 @@
       </c>
       <c r="N32" s="77"/>
     </row>
-    <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
         <v>122</v>
       </c>
@@ -6820,7 +6816,7 @@
       </c>
       <c r="N33" s="82"/>
     </row>
-    <row r="34" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
         <v>124</v>
       </c>
@@ -6842,7 +6838,7 @@
       </c>
       <c r="N34" s="83"/>
     </row>
-    <row r="35" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
         <v>128</v>
       </c>
@@ -6864,7 +6860,7 @@
       </c>
       <c r="N35" s="38"/>
     </row>
-    <row r="36" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
         <v>135</v>
       </c>
@@ -6882,7 +6878,7 @@
       </c>
       <c r="N36" s="40"/>
     </row>
-    <row r="37" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>137</v>
       </c>
@@ -6896,13 +6892,13 @@
       </c>
       <c r="N37" s="43"/>
     </row>
-    <row r="38" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
         <v>147</v>
       </c>
       <c r="B38" s="89"/>
     </row>
-    <row r="40" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>75</v>
       </c>
@@ -6925,7 +6921,7 @@
       <c r="M40" s="196"/>
       <c r="N40" s="196"/>
     </row>
-    <row r="41" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>77</v>
       </c>
@@ -6948,7 +6944,7 @@
       <c r="M41" s="68"/>
       <c r="N41" s="196"/>
     </row>
-    <row r="42" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>191</v>
       </c>
@@ -6971,7 +6967,7 @@
       <c r="M42" s="65"/>
       <c r="N42" s="196"/>
     </row>
-    <row r="43" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F43" s="24" t="s">
         <v>165</v>
       </c>
@@ -6981,52 +6977,52 @@
       <c r="N43" s="196"/>
       <c r="Q43" s="170"/>
     </row>
-    <row r="44" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L44" s="196"/>
       <c r="M44" s="43"/>
       <c r="N44" s="196"/>
       <c r="Q44" s="170"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="L45" s="196"/>
       <c r="M45" s="196"/>
       <c r="N45" s="196"/>
       <c r="Q45" s="170"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E47" s="170"/>
     </row>
-    <row r="48" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C48" s="24" t="s">
         <v>137</v>
       </c>
       <c r="D48" s="83"/>
     </row>
-    <row r="49" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C49" s="24" t="s">
         <v>79</v>
       </c>
       <c r="D49" s="59"/>
     </row>
-    <row r="50" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C50" s="24" t="s">
         <v>94</v>
       </c>
       <c r="D50" s="151"/>
     </row>
-    <row r="51" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C51" s="24" t="s">
         <v>6</v>
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C52" s="24" t="s">
         <v>191</v>
       </c>
       <c r="D52" s="40"/>
     </row>
-    <row r="53" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C53" s="24" t="s">
         <v>52</v>
       </c>
@@ -7036,7 +7032,7 @@
       </c>
       <c r="G53" s="23"/>
     </row>
-    <row r="54" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C54" s="24" t="s">
         <v>66</v>
       </c>
@@ -7046,7 +7042,7 @@
       </c>
       <c r="G54" s="29"/>
     </row>
-    <row r="55" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C55" s="24" t="s">
         <v>167</v>
       </c>
@@ -7057,7 +7053,7 @@
       <c r="G55" s="28"/>
       <c r="H55" s="170"/>
     </row>
-    <row r="56" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C56" s="24" t="s">
         <v>70</v>
       </c>
@@ -7065,7 +7061,7 @@
       <c r="F56" s="24"/>
       <c r="H56" s="170"/>
     </row>
-    <row r="57" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C57" s="24" t="s">
         <v>147</v>
       </c>
@@ -7079,7 +7075,7 @@
       </c>
       <c r="L57" s="8"/>
     </row>
-    <row r="58" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C58" s="24" t="s">
         <v>124</v>
       </c>
@@ -7094,7 +7090,7 @@
       <c r="L58" s="14"/>
       <c r="M58" s="170"/>
     </row>
-    <row r="59" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="K59" s="24" t="s">
         <v>191</v>
       </c>
@@ -7104,7 +7100,7 @@
       </c>
       <c r="P59" s="40"/>
     </row>
-    <row r="60" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C60" s="180" t="s">
         <v>417</v>
       </c>
@@ -7121,7 +7117,7 @@
       </c>
       <c r="P60" s="8"/>
     </row>
-    <row r="61" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C61" s="24" t="s">
         <v>167</v>
       </c>
@@ -7143,7 +7139,7 @@
       </c>
       <c r="P61" s="59"/>
     </row>
-    <row r="62" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C62" s="24" t="s">
         <v>139</v>
       </c>
@@ -7160,7 +7156,7 @@
       </c>
       <c r="P62" s="65"/>
     </row>
-    <row r="63" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C63" s="24" t="s">
         <v>94</v>
       </c>
@@ -7170,7 +7166,7 @@
       </c>
       <c r="M63" s="170"/>
     </row>
-    <row r="64" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C64" s="24" t="s">
         <v>191</v>
       </c>
@@ -7179,13 +7175,13 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="65" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I65" s="24" t="s">
         <v>147</v>
       </c>
       <c r="J65" s="89"/>
     </row>
-    <row r="66" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C66" s="24" t="s">
         <v>70</v>
       </c>
@@ -7196,7 +7192,7 @@
       </c>
       <c r="J66" s="84"/>
     </row>
-    <row r="67" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C67" s="24" t="s">
         <v>147</v>
       </c>
@@ -7207,7 +7203,7 @@
       </c>
       <c r="J67" s="151"/>
     </row>
-    <row r="68" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C68" s="24" t="s">
         <v>52</v>
       </c>
@@ -7222,7 +7218,7 @@
       </c>
       <c r="P68" s="54"/>
     </row>
-    <row r="69" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I69" s="24" t="s">
         <v>196</v>
       </c>
@@ -7238,7 +7234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I70" s="24" t="s">
         <v>191</v>
       </c>
@@ -7256,7 +7252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L71" s="24" t="s">
         <v>137</v>
       </c>
@@ -7265,7 +7261,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F72" s="24" t="s">
         <v>6</v>
       </c>
@@ -7282,7 +7278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F73" s="24" t="s">
         <v>139</v>
       </c>
@@ -7299,7 +7295,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F74" s="24" t="s">
         <v>94</v>
       </c>
@@ -7316,13 +7312,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L75" s="24" t="s">
         <v>191</v>
       </c>
       <c r="M75" s="40"/>
     </row>
-    <row r="76" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L76" s="24" t="s">
         <v>99</v>
       </c>
@@ -7331,7 +7327,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="77" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G77" s="24" t="s">
         <v>67</v>
       </c>
@@ -7344,7 +7340,7 @@
       </c>
       <c r="P77" s="83"/>
     </row>
-    <row r="78" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F78" s="24" t="s">
         <v>66</v>
       </c>
@@ -7364,7 +7360,7 @@
       </c>
       <c r="P78" s="77"/>
     </row>
-    <row r="79" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F79" s="24" t="s">
         <v>188</v>
       </c>
@@ -7381,7 +7377,7 @@
       </c>
       <c r="P79" s="80"/>
     </row>
-    <row r="80" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L80" s="24" t="s">
         <v>261</v>
       </c>
@@ -7391,7 +7387,7 @@
       </c>
       <c r="P80" s="54"/>
     </row>
-    <row r="81" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B81" s="184" t="s">
         <v>253</v>
       </c>
@@ -7421,7 +7417,7 @@
       </c>
       <c r="P81" s="52"/>
     </row>
-    <row r="82" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B82" s="187" t="s">
         <v>188</v>
       </c>
@@ -7451,7 +7447,7 @@
       </c>
       <c r="P82" s="151"/>
     </row>
-    <row r="83" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B83" s="188" t="s">
         <v>196</v>
       </c>
@@ -7481,7 +7477,7 @@
       </c>
       <c r="P83" s="66"/>
     </row>
-    <row r="84" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L84" s="24" t="s">
         <v>17</v>
       </c>
@@ -7491,7 +7487,7 @@
       </c>
       <c r="P84" s="15"/>
     </row>
-    <row r="85" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B85" s="183" t="s">
         <v>422</v>
       </c>
@@ -7504,7 +7500,7 @@
       </c>
       <c r="P85" s="9"/>
     </row>
-    <row r="86" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B86" s="24" t="s">
         <v>66</v>
       </c>
@@ -7524,7 +7520,7 @@
       </c>
       <c r="P86" s="23"/>
     </row>
-    <row r="87" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B87" s="24" t="s">
         <v>97</v>
       </c>
@@ -7544,7 +7540,7 @@
       </c>
       <c r="P87" s="40"/>
     </row>
-    <row r="88" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B88" s="24" t="s">
         <v>141</v>
       </c>
@@ -7560,7 +7556,7 @@
       </c>
       <c r="P88" s="43"/>
     </row>
-    <row r="89" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B89" s="24" t="s">
         <v>8</v>
       </c>
@@ -7576,7 +7572,7 @@
       </c>
       <c r="P89" s="127"/>
     </row>
-    <row r="90" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B90" s="24" t="s">
         <v>188</v>
       </c>
@@ -7588,7 +7584,7 @@
       </c>
       <c r="E90" s="39"/>
     </row>
-    <row r="91" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B91" s="24" t="s">
         <v>253</v>
       </c>
@@ -7600,7 +7596,7 @@
       </c>
       <c r="E91" s="88"/>
     </row>
-    <row r="92" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B92" s="24" t="s">
         <v>196</v>
       </c>
@@ -7612,7 +7608,7 @@
       </c>
       <c r="E92" s="43"/>
     </row>
-    <row r="93" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B93" s="24" t="s">
         <v>79</v>
       </c>
@@ -7624,7 +7620,7 @@
       </c>
       <c r="E93" s="59"/>
     </row>
-    <row r="94" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B94" s="24" t="s">
         <v>62</v>
       </c>
@@ -7636,167 +7632,167 @@
       </c>
       <c r="E94" s="52"/>
     </row>
-    <row r="122" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E122" s="24"/>
       <c r="F122" s="24"/>
       <c r="G122" s="170"/>
     </row>
-    <row r="123" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E123" s="24"/>
       <c r="F123" s="24"/>
       <c r="G123" s="170"/>
     </row>
-    <row r="124" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E124" s="24"/>
       <c r="F124" s="24"/>
       <c r="G124" s="170"/>
     </row>
-    <row r="125" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E125" s="24"/>
       <c r="F125" s="24"/>
       <c r="G125" s="170"/>
     </row>
-    <row r="130" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I130" s="24"/>
       <c r="J130" s="170"/>
     </row>
-    <row r="131" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I131" s="24"/>
       <c r="J131" s="170"/>
     </row>
-    <row r="132" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I132" s="24"/>
       <c r="J132" s="170"/>
     </row>
-    <row r="133" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I133" s="24"/>
       <c r="J133" s="170"/>
     </row>
-    <row r="134" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I134" s="24"/>
       <c r="J134" s="170"/>
     </row>
-    <row r="135" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I135" s="24"/>
       <c r="J135" s="170"/>
     </row>
-    <row r="136" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I136" s="24"/>
       <c r="J136" s="170"/>
     </row>
-    <row r="137" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I137" s="24"/>
       <c r="J137" s="207"/>
     </row>
-    <row r="138" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I138" s="24"/>
       <c r="J138" s="207"/>
     </row>
-    <row r="139" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I139" s="24"/>
       <c r="J139" s="207"/>
     </row>
-    <row r="140" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I140" s="24"/>
       <c r="J140" s="170"/>
     </row>
-    <row r="141" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I141" s="24"/>
       <c r="J141" s="170"/>
     </row>
-    <row r="142" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I142" s="24"/>
       <c r="J142" s="170"/>
     </row>
-    <row r="143" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I143" s="24"/>
       <c r="J143" s="170"/>
     </row>
-    <row r="144" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I144" s="24"/>
       <c r="J144" s="170"/>
     </row>
-    <row r="145" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I145" s="24"/>
       <c r="J145" s="170"/>
     </row>
-    <row r="146" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I146" s="24"/>
       <c r="J146" s="170"/>
     </row>
-    <row r="147" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I147" s="24"/>
       <c r="J147" s="170"/>
     </row>
-    <row r="148" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I148" s="24"/>
       <c r="J148" s="170"/>
     </row>
-    <row r="149" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I149" s="24"/>
       <c r="J149" s="170"/>
     </row>
-    <row r="150" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I150" s="24"/>
       <c r="J150" s="170"/>
     </row>
-    <row r="151" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I151" s="24"/>
       <c r="J151" s="170"/>
     </row>
-    <row r="152" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I152" s="24"/>
       <c r="J152" s="24"/>
     </row>
-    <row r="153" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I153" s="24"/>
       <c r="J153" s="24"/>
     </row>
-    <row r="154" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I154" s="24"/>
       <c r="J154" s="24"/>
     </row>
-    <row r="155" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I155" s="24"/>
       <c r="J155" s="24"/>
     </row>
-    <row r="156" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I156" s="24"/>
       <c r="J156" s="170"/>
     </row>
-    <row r="157" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I157" s="24"/>
       <c r="J157" s="24"/>
     </row>
-    <row r="158" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I158" s="24"/>
       <c r="J158" s="24"/>
     </row>
-    <row r="159" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I159" s="24"/>
       <c r="J159" s="24"/>
     </row>
-    <row r="160" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I160" s="24"/>
       <c r="J160" s="170"/>
     </row>
-    <row r="161" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I161" s="24"/>
       <c r="J161" s="170"/>
     </row>
-    <row r="162" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I162" s="24"/>
       <c r="J162" s="170"/>
     </row>
-    <row r="163" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I163" s="24"/>
       <c r="J163" s="170"/>
     </row>
-    <row r="164" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I164" s="24"/>
       <c r="J164" s="170"/>
     </row>
-    <row r="165" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I165" s="24"/>
       <c r="J165" s="170"/>
     </row>

</xml_diff>

<commit_message>
becca workspace and aggression updates
</commit_message>
<xml_diff>
--- a/Functions and Code/Color Palette.xlsx
+++ b/Functions and Code/Color Palette.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evyndickinson/Documents/matlabroot/Functions and Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yaleedu-my.sharepoint.com/personal/rebecca_ray_yale_edu/Documents/Documents/GitHub/matlabroot/Functions and Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6EC13C-3921-7244-9FEF-4BB8A6C03E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="580" windowWidth="29920" windowHeight="18760" xr2:uid="{B90EF345-F11D-4BE8-9704-8686C964E4D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B90EF345-F11D-4BE8-9704-8686C964E4D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4044,25 +4044,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBF5F8C-DD5F-4ED3-9E54-88EB7CF98784}">
   <dimension ref="A1:D195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E168" sqref="E168"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="170" customWidth="1"/>
-    <col min="4" max="4" width="6.5" style="24" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.6640625" customWidth="1"/>
-    <col min="20" max="20" width="19.83203125" customWidth="1"/>
-    <col min="23" max="23" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="170" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" style="24" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.7109375" customWidth="1"/>
+    <col min="20" max="20" width="19.85546875" customWidth="1"/>
+    <col min="23" max="23" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="162" t="s">
         <v>305</v>
       </c>
@@ -4070,7 +4070,7 @@
       <c r="C1" s="169"/>
       <c r="D1" s="164"/>
     </row>
-    <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
         <v>54</v>
       </c>
@@ -4082,7 +4082,7 @@
       </c>
       <c r="D2" s="48"/>
     </row>
-    <row r="3" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>56</v>
       </c>
@@ -4094,7 +4094,7 @@
       </c>
       <c r="D3" s="49"/>
     </row>
-    <row r="4" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>58</v>
       </c>
@@ -4106,7 +4106,7 @@
       </c>
       <c r="D4" s="50"/>
     </row>
-    <row r="5" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
         <v>60</v>
       </c>
@@ -4118,7 +4118,7 @@
       </c>
       <c r="D5" s="51"/>
     </row>
-    <row r="6" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>62</v>
       </c>
@@ -4130,7 +4130,7 @@
       </c>
       <c r="D6" s="52"/>
     </row>
-    <row r="7" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
         <v>64</v>
       </c>
@@ -4142,7 +4142,7 @@
       </c>
       <c r="D7" s="53"/>
     </row>
-    <row r="8" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
         <v>66</v>
       </c>
@@ -4154,7 +4154,7 @@
       </c>
       <c r="D8" s="54"/>
     </row>
-    <row r="9" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
         <v>68</v>
       </c>
@@ -4166,7 +4166,7 @@
       </c>
       <c r="D9" s="55"/>
     </row>
-    <row r="10" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
         <v>70</v>
       </c>
@@ -4178,7 +4178,7 @@
       </c>
       <c r="D10" s="152"/>
     </row>
-    <row r="11" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="159" t="s">
         <v>72</v>
       </c>
@@ -4186,7 +4186,7 @@
       <c r="C11" s="171"/>
       <c r="D11" s="161"/>
     </row>
-    <row r="12" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>73</v>
       </c>
@@ -4198,7 +4198,7 @@
       </c>
       <c r="D12" s="56"/>
     </row>
-    <row r="13" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>75</v>
       </c>
@@ -4210,7 +4210,7 @@
       </c>
       <c r="D13" s="57"/>
     </row>
-    <row r="14" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>77</v>
       </c>
@@ -4222,7 +4222,7 @@
       </c>
       <c r="D14" s="58"/>
     </row>
-    <row r="15" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
         <v>79</v>
       </c>
@@ -4234,7 +4234,7 @@
       </c>
       <c r="D15" s="59"/>
     </row>
-    <row r="16" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
         <v>81</v>
       </c>
@@ -4246,7 +4246,7 @@
       </c>
       <c r="D16" s="60"/>
     </row>
-    <row r="17" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>83</v>
       </c>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="D17" s="165"/>
     </row>
-    <row r="18" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="167" t="s">
         <v>85</v>
       </c>
@@ -4266,7 +4266,7 @@
       <c r="C18" s="172"/>
       <c r="D18" s="166"/>
     </row>
-    <row r="19" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
         <v>86</v>
       </c>
@@ -4278,7 +4278,7 @@
       </c>
       <c r="D19" s="61"/>
     </row>
-    <row r="20" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
         <v>88</v>
       </c>
@@ -4290,7 +4290,7 @@
       </c>
       <c r="D20" s="62"/>
     </row>
-    <row r="21" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>90</v>
       </c>
@@ -4302,7 +4302,7 @@
       </c>
       <c r="D21" s="63"/>
     </row>
-    <row r="22" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>92</v>
       </c>
@@ -4314,7 +4314,7 @@
       </c>
       <c r="D22" s="64"/>
     </row>
-    <row r="23" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>94</v>
       </c>
@@ -4326,7 +4326,7 @@
       </c>
       <c r="D23" s="151"/>
     </row>
-    <row r="24" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="156" t="s">
         <v>96</v>
       </c>
@@ -4334,7 +4334,7 @@
       <c r="C24" s="173"/>
       <c r="D24" s="158"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>97</v>
       </c>
@@ -4346,7 +4346,7 @@
       </c>
       <c r="D25" s="65"/>
     </row>
-    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
         <v>99</v>
       </c>
@@ -4358,7 +4358,7 @@
       </c>
       <c r="D26" s="66"/>
     </row>
-    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
         <v>101</v>
       </c>
@@ -4370,7 +4370,7 @@
       </c>
       <c r="D27" s="67"/>
     </row>
-    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
         <v>103</v>
       </c>
@@ -4382,7 +4382,7 @@
       </c>
       <c r="D28" s="68"/>
     </row>
-    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
         <v>105</v>
       </c>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="D29" s="69"/>
     </row>
-    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="s">
         <v>107</v>
       </c>
@@ -4406,7 +4406,7 @@
       </c>
       <c r="D30" s="70"/>
     </row>
-    <row r="31" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="s">
         <v>109</v>
       </c>
@@ -4418,7 +4418,7 @@
       </c>
       <c r="D31" s="71"/>
     </row>
-    <row r="32" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>111</v>
       </c>
@@ -4430,7 +4430,7 @@
       </c>
       <c r="D32" s="72"/>
     </row>
-    <row r="33" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="24" t="s">
         <v>113</v>
       </c>
@@ -4442,7 +4442,7 @@
       </c>
       <c r="D33" s="73"/>
     </row>
-    <row r="34" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>115</v>
       </c>
@@ -4454,7 +4454,7 @@
       </c>
       <c r="D34" s="74"/>
     </row>
-    <row r="35" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="24" t="s">
         <v>117</v>
       </c>
@@ -4466,7 +4466,7 @@
       </c>
       <c r="D35" s="150"/>
     </row>
-    <row r="36" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="153" t="s">
         <v>119</v>
       </c>
@@ -4474,7 +4474,7 @@
       <c r="C36" s="174"/>
       <c r="D36" s="155"/>
     </row>
-    <row r="37" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="24" t="s">
         <v>120</v>
       </c>
@@ -4486,7 +4486,7 @@
       </c>
       <c r="D37" s="75"/>
     </row>
-    <row r="38" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="24" t="s">
         <v>122</v>
       </c>
@@ -4498,7 +4498,7 @@
       </c>
       <c r="D38" s="76"/>
     </row>
-    <row r="39" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="24" t="s">
         <v>124</v>
       </c>
@@ -4510,7 +4510,7 @@
       </c>
       <c r="D39" s="77"/>
     </row>
-    <row r="40" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="24" t="s">
         <v>126</v>
       </c>
@@ -4522,7 +4522,7 @@
       </c>
       <c r="D40" s="78"/>
     </row>
-    <row r="41" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="24" t="s">
         <v>128</v>
       </c>
@@ -4534,7 +4534,7 @@
       </c>
       <c r="D41" s="79"/>
     </row>
-    <row r="42" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="24" t="s">
         <v>130</v>
       </c>
@@ -4546,7 +4546,7 @@
       </c>
       <c r="D42" s="80"/>
     </row>
-    <row r="43" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="24" t="s">
         <v>132</v>
       </c>
@@ -4558,7 +4558,7 @@
       </c>
       <c r="D43" s="80"/>
     </row>
-    <row r="44" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="24" t="s">
         <v>133</v>
       </c>
@@ -4570,7 +4570,7 @@
       </c>
       <c r="D44" s="81"/>
     </row>
-    <row r="45" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="24" t="s">
         <v>135</v>
       </c>
@@ -4582,7 +4582,7 @@
       </c>
       <c r="D45" s="82"/>
     </row>
-    <row r="46" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="24" t="s">
         <v>137</v>
       </c>
@@ -4594,7 +4594,7 @@
       </c>
       <c r="D46" s="83"/>
     </row>
-    <row r="47" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="24" t="s">
         <v>139</v>
       </c>
@@ -4606,7 +4606,7 @@
       </c>
       <c r="D47" s="84"/>
     </row>
-    <row r="48" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
         <v>141</v>
       </c>
@@ -4618,7 +4618,7 @@
       </c>
       <c r="D48" s="85"/>
     </row>
-    <row r="49" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="24" t="s">
         <v>143</v>
       </c>
@@ -4630,7 +4630,7 @@
       </c>
       <c r="D49" s="86"/>
     </row>
-    <row r="50" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="24" t="s">
         <v>145</v>
       </c>
@@ -4642,7 +4642,7 @@
       </c>
       <c r="D50" s="87"/>
     </row>
-    <row r="51" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="24" t="s">
         <v>146</v>
       </c>
@@ -4654,7 +4654,7 @@
       </c>
       <c r="D51" s="88"/>
     </row>
-    <row r="52" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="24" t="s">
         <v>147</v>
       </c>
@@ -4666,7 +4666,7 @@
       </c>
       <c r="D52" s="89"/>
     </row>
-    <row r="53" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="24" t="s">
         <v>149</v>
       </c>
@@ -4678,7 +4678,7 @@
       </c>
       <c r="D53" s="90"/>
     </row>
-    <row r="54" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="24" t="s">
         <v>151</v>
       </c>
@@ -4690,7 +4690,7 @@
       </c>
       <c r="D54" s="91"/>
     </row>
-    <row r="55" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="24" t="s">
         <v>153</v>
       </c>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="D55" s="92"/>
     </row>
-    <row r="56" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="147" t="s">
         <v>155</v>
       </c>
@@ -4710,7 +4710,7 @@
       <c r="C56" s="175"/>
       <c r="D56" s="149"/>
     </row>
-    <row r="57" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="24" t="s">
         <v>0</v>
       </c>
@@ -4722,7 +4722,7 @@
       </c>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="24" t="s">
         <v>2</v>
       </c>
@@ -4734,7 +4734,7 @@
       </c>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="24" t="s">
         <v>4</v>
       </c>
@@ -4746,7 +4746,7 @@
       </c>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="24" t="s">
         <v>6</v>
       </c>
@@ -4758,7 +4758,7 @@
       </c>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="24" t="s">
         <v>8</v>
       </c>
@@ -4770,7 +4770,7 @@
       </c>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="24" t="s">
         <v>10</v>
       </c>
@@ -4782,7 +4782,7 @@
       </c>
       <c r="D62" s="6"/>
     </row>
-    <row r="63" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="24" t="s">
         <v>12</v>
       </c>
@@ -4794,7 +4794,7 @@
       </c>
       <c r="D63" s="7"/>
     </row>
-    <row r="64" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="24" t="s">
         <v>14</v>
       </c>
@@ -4806,7 +4806,7 @@
       </c>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="24" t="s">
         <v>17</v>
       </c>
@@ -4818,7 +4818,7 @@
       </c>
       <c r="D65" s="9"/>
     </row>
-    <row r="66" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="24" t="s">
         <v>20</v>
       </c>
@@ -4830,7 +4830,7 @@
       </c>
       <c r="D66" s="10"/>
     </row>
-    <row r="67" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="24" t="s">
         <v>22</v>
       </c>
@@ -4842,7 +4842,7 @@
       </c>
       <c r="D67" s="11"/>
     </row>
-    <row r="68" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="24" t="s">
         <v>25</v>
       </c>
@@ -4854,7 +4854,7 @@
       </c>
       <c r="D68" s="12"/>
     </row>
-    <row r="69" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="24" t="s">
         <v>28</v>
       </c>
@@ -4866,7 +4866,7 @@
       </c>
       <c r="D69" s="13"/>
     </row>
-    <row r="70" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="24" t="s">
         <v>30</v>
       </c>
@@ -4878,7 +4878,7 @@
       </c>
       <c r="D70" s="14"/>
     </row>
-    <row r="71" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="24" t="s">
         <v>32</v>
       </c>
@@ -4890,7 +4890,7 @@
       </c>
       <c r="D71" s="15"/>
     </row>
-    <row r="72" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
         <v>35</v>
       </c>
@@ -4902,7 +4902,7 @@
       </c>
       <c r="D72" s="16"/>
     </row>
-    <row r="73" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="24" t="s">
         <v>38</v>
       </c>
@@ -4914,7 +4914,7 @@
       </c>
       <c r="D73" s="17"/>
     </row>
-    <row r="74" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="24" t="s">
         <v>40</v>
       </c>
@@ -4926,7 +4926,7 @@
       </c>
       <c r="D74" s="18"/>
     </row>
-    <row r="75" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="24" t="s">
         <v>43</v>
       </c>
@@ -4938,7 +4938,7 @@
       </c>
       <c r="D75" s="19"/>
     </row>
-    <row r="76" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="24" t="s">
         <v>45</v>
       </c>
@@ -4950,7 +4950,7 @@
       </c>
       <c r="D76" s="20"/>
     </row>
-    <row r="77" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="24" t="s">
         <v>47</v>
       </c>
@@ -4962,7 +4962,7 @@
       </c>
       <c r="D77" s="21"/>
     </row>
-    <row r="78" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="24" t="s">
         <v>49</v>
       </c>
@@ -4974,7 +4974,7 @@
       </c>
       <c r="D78" s="22"/>
     </row>
-    <row r="79" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="24" t="s">
         <v>52</v>
       </c>
@@ -4986,7 +4986,7 @@
       </c>
       <c r="D79" s="23"/>
     </row>
-    <row r="80" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="144" t="s">
         <v>156</v>
       </c>
@@ -4994,7 +4994,7 @@
       <c r="C80" s="176"/>
       <c r="D80" s="146"/>
     </row>
-    <row r="81" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="24" t="s">
         <v>157</v>
       </c>
@@ -5006,7 +5006,7 @@
       </c>
       <c r="D81" s="25"/>
     </row>
-    <row r="82" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="24" t="s">
         <v>160</v>
       </c>
@@ -5018,7 +5018,7 @@
       </c>
       <c r="D82" s="25"/>
     </row>
-    <row r="83" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="24" t="s">
         <v>161</v>
       </c>
@@ -5030,7 +5030,7 @@
       </c>
       <c r="D83" s="26"/>
     </row>
-    <row r="84" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="24" t="s">
         <v>163</v>
       </c>
@@ -5042,7 +5042,7 @@
       </c>
       <c r="D84" s="27"/>
     </row>
-    <row r="85" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="24" t="s">
         <v>165</v>
       </c>
@@ -5054,7 +5054,7 @@
       </c>
       <c r="D85" s="28"/>
     </row>
-    <row r="86" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="24" t="s">
         <v>167</v>
       </c>
@@ -5066,7 +5066,7 @@
       </c>
       <c r="D86" s="29"/>
     </row>
-    <row r="87" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="24" t="s">
         <v>169</v>
       </c>
@@ -5078,7 +5078,7 @@
       </c>
       <c r="D87" s="30"/>
     </row>
-    <row r="88" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="24" t="s">
         <v>171</v>
       </c>
@@ -5090,7 +5090,7 @@
       </c>
       <c r="D88" s="31"/>
     </row>
-    <row r="89" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="24" t="s">
         <v>174</v>
       </c>
@@ -5102,7 +5102,7 @@
       </c>
       <c r="D89" s="32"/>
     </row>
-    <row r="90" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="24" t="s">
         <v>176</v>
       </c>
@@ -5114,7 +5114,7 @@
       </c>
       <c r="D90" s="33"/>
     </row>
-    <row r="91" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="24" t="s">
         <v>178</v>
       </c>
@@ -5126,7 +5126,7 @@
       </c>
       <c r="D91" s="34"/>
     </row>
-    <row r="92" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="24" t="s">
         <v>180</v>
       </c>
@@ -5138,7 +5138,7 @@
       </c>
       <c r="D92" s="35"/>
     </row>
-    <row r="93" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="24" t="s">
         <v>182</v>
       </c>
@@ -5150,7 +5150,7 @@
       </c>
       <c r="D93" s="36"/>
     </row>
-    <row r="94" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="24" t="s">
         <v>184</v>
       </c>
@@ -5162,7 +5162,7 @@
       </c>
       <c r="D94" s="37"/>
     </row>
-    <row r="95" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="24" t="s">
         <v>186</v>
       </c>
@@ -5174,7 +5174,7 @@
       </c>
       <c r="D95" s="38"/>
     </row>
-    <row r="96" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="24" t="s">
         <v>188</v>
       </c>
@@ -5186,7 +5186,7 @@
       </c>
       <c r="D96" s="39"/>
     </row>
-    <row r="97" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="24" t="s">
         <v>191</v>
       </c>
@@ -5198,7 +5198,7 @@
       </c>
       <c r="D97" s="40"/>
     </row>
-    <row r="98" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="24" t="s">
         <v>193</v>
       </c>
@@ -5210,7 +5210,7 @@
       </c>
       <c r="D98" s="41"/>
     </row>
-    <row r="99" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="24" t="s">
         <v>195</v>
       </c>
@@ -5222,7 +5222,7 @@
       </c>
       <c r="D99" s="42"/>
     </row>
-    <row r="100" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="24" t="s">
         <v>196</v>
       </c>
@@ -5234,7 +5234,7 @@
       </c>
       <c r="D100" s="43"/>
     </row>
-    <row r="101" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="24" t="s">
         <v>199</v>
       </c>
@@ -5246,7 +5246,7 @@
       </c>
       <c r="D101" s="44"/>
     </row>
-    <row r="102" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="24" t="s">
         <v>202</v>
       </c>
@@ -5258,7 +5258,7 @@
       </c>
       <c r="D102" s="45"/>
     </row>
-    <row r="103" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="24" t="s">
         <v>205</v>
       </c>
@@ -5270,7 +5270,7 @@
       </c>
       <c r="D103" s="46"/>
     </row>
-    <row r="104" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="24" t="s">
         <v>207</v>
       </c>
@@ -5282,7 +5282,7 @@
       </c>
       <c r="D104" s="47"/>
     </row>
-    <row r="105" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="141" t="s">
         <v>209</v>
       </c>
@@ -5290,7 +5290,7 @@
       <c r="C105" s="177"/>
       <c r="D105" s="143"/>
     </row>
-    <row r="106" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="24" t="s">
         <v>210</v>
       </c>
@@ -5302,7 +5302,7 @@
       </c>
       <c r="D106" s="93"/>
     </row>
-    <row r="107" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="24" t="s">
         <v>212</v>
       </c>
@@ -5314,7 +5314,7 @@
       </c>
       <c r="D107" s="94"/>
     </row>
-    <row r="108" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="24" t="s">
         <v>214</v>
       </c>
@@ -5326,7 +5326,7 @@
       </c>
       <c r="D108" s="95"/>
     </row>
-    <row r="109" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="24" t="s">
         <v>216</v>
       </c>
@@ -5338,7 +5338,7 @@
       </c>
       <c r="D109" s="96"/>
     </row>
-    <row r="110" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="24" t="s">
         <v>218</v>
       </c>
@@ -5350,7 +5350,7 @@
       </c>
       <c r="D110" s="97"/>
     </row>
-    <row r="111" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="24" t="s">
         <v>220</v>
       </c>
@@ -5362,7 +5362,7 @@
       </c>
       <c r="D111" s="98"/>
     </row>
-    <row r="112" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="24" t="s">
         <v>222</v>
       </c>
@@ -5374,7 +5374,7 @@
       </c>
       <c r="D112" s="99"/>
     </row>
-    <row r="113" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="24" t="s">
         <v>224</v>
       </c>
@@ -5386,7 +5386,7 @@
       </c>
       <c r="D113" s="100"/>
     </row>
-    <row r="114" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="24" t="s">
         <v>226</v>
       </c>
@@ -5398,7 +5398,7 @@
       </c>
       <c r="D114" s="101"/>
     </row>
-    <row r="115" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="24" t="s">
         <v>229</v>
       </c>
@@ -5410,7 +5410,7 @@
       </c>
       <c r="D115" s="102"/>
     </row>
-    <row r="116" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
         <v>232</v>
       </c>
@@ -5422,7 +5422,7 @@
       </c>
       <c r="D116" s="103"/>
     </row>
-    <row r="117" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="24" t="s">
         <v>235</v>
       </c>
@@ -5434,7 +5434,7 @@
       </c>
       <c r="D117" s="104"/>
     </row>
-    <row r="118" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="24" t="s">
         <v>238</v>
       </c>
@@ -5446,7 +5446,7 @@
       </c>
       <c r="D118" s="105"/>
     </row>
-    <row r="119" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="24" t="s">
         <v>241</v>
       </c>
@@ -5458,7 +5458,7 @@
       </c>
       <c r="D119" s="106"/>
     </row>
-    <row r="120" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="24" t="s">
         <v>244</v>
       </c>
@@ -5470,7 +5470,7 @@
       </c>
       <c r="D120" s="107"/>
     </row>
-    <row r="121" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="24" t="s">
         <v>247</v>
       </c>
@@ -5482,7 +5482,7 @@
       </c>
       <c r="D121" s="108"/>
     </row>
-    <row r="122" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="24" t="s">
         <v>250</v>
       </c>
@@ -5494,7 +5494,7 @@
       </c>
       <c r="D122" s="132"/>
     </row>
-    <row r="123" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="135" t="s">
         <v>252</v>
       </c>
@@ -5502,7 +5502,7 @@
       <c r="C123" s="178"/>
       <c r="D123" s="134"/>
     </row>
-    <row r="124" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="24" t="s">
         <v>253</v>
       </c>
@@ -5514,7 +5514,7 @@
       </c>
       <c r="D124" s="88"/>
     </row>
-    <row r="125" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="24" t="s">
         <v>255</v>
       </c>
@@ -5526,7 +5526,7 @@
       </c>
       <c r="D125" s="109"/>
     </row>
-    <row r="126" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="24" t="s">
         <v>257</v>
       </c>
@@ -5538,7 +5538,7 @@
       </c>
       <c r="D126" s="110"/>
     </row>
-    <row r="127" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="24" t="s">
         <v>259</v>
       </c>
@@ -5550,7 +5550,7 @@
       </c>
       <c r="D127" s="111"/>
     </row>
-    <row r="128" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="24" t="s">
         <v>261</v>
       </c>
@@ -5562,7 +5562,7 @@
       </c>
       <c r="D128" s="112"/>
     </row>
-    <row r="129" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="24" t="s">
         <v>263</v>
       </c>
@@ -5574,7 +5574,7 @@
       </c>
       <c r="D129" s="113"/>
     </row>
-    <row r="130" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="24" t="s">
         <v>265</v>
       </c>
@@ -5586,7 +5586,7 @@
       </c>
       <c r="D130" s="114"/>
     </row>
-    <row r="131" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="24" t="s">
         <v>267</v>
       </c>
@@ -5598,7 +5598,7 @@
       </c>
       <c r="D131" s="115"/>
     </row>
-    <row r="132" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="24" t="s">
         <v>269</v>
       </c>
@@ -5610,7 +5610,7 @@
       </c>
       <c r="D132" s="116"/>
     </row>
-    <row r="133" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="24" t="s">
         <v>271</v>
       </c>
@@ -5622,7 +5622,7 @@
       </c>
       <c r="D133" s="117"/>
     </row>
-    <row r="134" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="24" t="s">
         <v>273</v>
       </c>
@@ -5634,7 +5634,7 @@
       </c>
       <c r="D134" s="118"/>
     </row>
-    <row r="135" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="24" t="s">
         <v>275</v>
       </c>
@@ -5646,7 +5646,7 @@
       </c>
       <c r="D135" s="119"/>
     </row>
-    <row r="136" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="24" t="s">
         <v>277</v>
       </c>
@@ -5658,7 +5658,7 @@
       </c>
       <c r="D136" s="120"/>
     </row>
-    <row r="137" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="24" t="s">
         <v>279</v>
       </c>
@@ -5670,7 +5670,7 @@
       </c>
       <c r="D137" s="121"/>
     </row>
-    <row r="138" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="24" t="s">
         <v>281</v>
       </c>
@@ -5682,7 +5682,7 @@
       </c>
       <c r="D138" s="122"/>
     </row>
-    <row r="139" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="24" t="s">
         <v>283</v>
       </c>
@@ -5694,7 +5694,7 @@
       </c>
       <c r="D139" s="123"/>
     </row>
-    <row r="140" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="24" t="s">
         <v>285</v>
       </c>
@@ -5706,7 +5706,7 @@
       </c>
       <c r="D140" s="136"/>
     </row>
-    <row r="141" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="138" t="s">
         <v>287</v>
       </c>
@@ -5714,7 +5714,7 @@
       <c r="C141" s="179"/>
       <c r="D141" s="140"/>
     </row>
-    <row r="142" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="24" t="s">
         <v>288</v>
       </c>
@@ -5726,7 +5726,7 @@
       </c>
       <c r="D142" s="124"/>
     </row>
-    <row r="143" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="24" t="s">
         <v>290</v>
       </c>
@@ -5738,7 +5738,7 @@
       </c>
       <c r="D143" s="125"/>
     </row>
-    <row r="144" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="24" t="s">
         <v>292</v>
       </c>
@@ -5750,7 +5750,7 @@
       </c>
       <c r="D144" s="125"/>
     </row>
-    <row r="145" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="24" t="s">
         <v>293</v>
       </c>
@@ -5762,7 +5762,7 @@
       </c>
       <c r="D145" s="126"/>
     </row>
-    <row r="146" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="24" t="s">
         <v>295</v>
       </c>
@@ -5774,7 +5774,7 @@
       </c>
       <c r="D146" s="127"/>
     </row>
-    <row r="147" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="24" t="s">
         <v>543</v>
       </c>
@@ -5786,7 +5786,7 @@
       </c>
       <c r="D147" s="128"/>
     </row>
-    <row r="148" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="24" t="s">
         <v>297</v>
       </c>
@@ -5798,7 +5798,7 @@
       </c>
       <c r="D148" s="128"/>
     </row>
-    <row r="149" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="24" t="s">
         <v>298</v>
       </c>
@@ -5810,7 +5810,7 @@
       </c>
       <c r="D149" s="129"/>
     </row>
-    <row r="150" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="24" t="s">
         <v>299</v>
       </c>
@@ -5822,7 +5822,7 @@
       </c>
       <c r="D150" s="130"/>
     </row>
-    <row r="151" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="24" t="s">
         <v>300</v>
       </c>
@@ -5834,7 +5834,7 @@
       </c>
       <c r="D151" s="131"/>
     </row>
-    <row r="152" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="24" t="s">
         <v>301</v>
       </c>
@@ -5846,7 +5846,7 @@
       </c>
       <c r="D152" s="197"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="24" t="s">
         <v>303</v>
       </c>
@@ -5858,7 +5858,7 @@
       </c>
       <c r="D153" s="198"/>
     </row>
-    <row r="154" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="199" t="s">
         <v>443</v>
       </c>
@@ -5866,7 +5866,7 @@
       <c r="C154" s="200"/>
       <c r="D154" s="199"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="24" t="s">
         <v>427</v>
       </c>
@@ -5878,7 +5878,7 @@
       </c>
       <c r="D155" s="201"/>
     </row>
-    <row r="156" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="24" t="s">
         <v>436</v>
       </c>
@@ -5890,7 +5890,7 @@
       </c>
       <c r="D156" s="205"/>
     </row>
-    <row r="157" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="24" t="s">
         <v>437</v>
       </c>
@@ -5902,7 +5902,7 @@
       </c>
       <c r="D157" s="202"/>
     </row>
-    <row r="158" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="24" t="s">
         <v>438</v>
       </c>
@@ -5914,7 +5914,7 @@
       </c>
       <c r="D158" s="203"/>
     </row>
-    <row r="159" spans="1:4" ht="21" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A159" s="24" t="s">
         <v>439</v>
       </c>
@@ -5926,7 +5926,7 @@
       </c>
       <c r="D159" s="204"/>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="24" t="s">
         <v>442</v>
       </c>
@@ -5938,7 +5938,7 @@
       </c>
       <c r="D160" s="206"/>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="24" t="s">
         <v>448</v>
       </c>
@@ -5950,7 +5950,7 @@
       </c>
       <c r="D161" s="208"/>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="24" t="s">
         <v>449</v>
       </c>
@@ -5962,7 +5962,7 @@
       </c>
       <c r="D162" s="209"/>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="24" t="s">
         <v>450</v>
       </c>
@@ -5974,7 +5974,7 @@
       </c>
       <c r="D163" s="210"/>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="24" t="s">
         <v>451</v>
       </c>
@@ -5986,7 +5986,7 @@
       </c>
       <c r="D164" s="211"/>
     </row>
-    <row r="165" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="199" t="s">
         <v>506</v>
       </c>
@@ -5994,7 +5994,7 @@
       <c r="C165" s="199"/>
       <c r="D165" s="199"/>
     </row>
-    <row r="166" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="24" t="s">
         <v>520</v>
       </c>
@@ -6006,7 +6006,7 @@
       </c>
       <c r="D166" s="234"/>
     </row>
-    <row r="167" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="24" t="s">
         <v>521</v>
       </c>
@@ -6018,7 +6018,7 @@
       </c>
       <c r="D167" s="230"/>
     </row>
-    <row r="168" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="24" t="s">
         <v>519</v>
       </c>
@@ -6030,7 +6030,7 @@
       </c>
       <c r="D168" s="231"/>
     </row>
-    <row r="169" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="24" t="s">
         <v>517</v>
       </c>
@@ -6042,7 +6042,7 @@
       </c>
       <c r="D169" s="232"/>
     </row>
-    <row r="170" spans="1:4" ht="21" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A170" s="24" t="s">
         <v>518</v>
       </c>
@@ -6054,7 +6054,7 @@
       </c>
       <c r="D170" s="233"/>
     </row>
-    <row r="171" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="199" t="s">
         <v>458</v>
       </c>
@@ -6062,7 +6062,7 @@
       <c r="C171" s="199"/>
       <c r="D171" s="199"/>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="24" t="s">
         <v>472</v>
       </c>
@@ -6074,7 +6074,7 @@
       </c>
       <c r="D172" s="215"/>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="24" t="s">
         <v>471</v>
       </c>
@@ -6086,7 +6086,7 @@
       </c>
       <c r="D173" s="217"/>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="24" t="s">
         <v>470</v>
       </c>
@@ -6098,7 +6098,7 @@
       </c>
       <c r="D174" s="218"/>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="24" t="s">
         <v>469</v>
       </c>
@@ -6110,7 +6110,7 @@
       </c>
       <c r="D175" s="219"/>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="24" t="s">
         <v>473</v>
       </c>
@@ -6122,7 +6122,7 @@
       </c>
       <c r="D176" s="220"/>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="24" t="s">
         <v>476</v>
       </c>
@@ -6134,7 +6134,7 @@
       </c>
       <c r="D177" s="216"/>
     </row>
-    <row r="178" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="199" t="s">
         <v>477</v>
       </c>
@@ -6142,7 +6142,7 @@
       <c r="C178" s="199"/>
       <c r="D178" s="199"/>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="24" t="s">
         <v>488</v>
       </c>
@@ -6154,7 +6154,7 @@
       </c>
       <c r="D179" s="221"/>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="24" t="s">
         <v>489</v>
       </c>
@@ -6166,7 +6166,7 @@
       </c>
       <c r="D180" s="222"/>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="24" t="s">
         <v>490</v>
       </c>
@@ -6178,7 +6178,7 @@
       </c>
       <c r="D181" s="223"/>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="24" t="s">
         <v>491</v>
       </c>
@@ -6190,7 +6190,7 @@
       </c>
       <c r="D182" s="224"/>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="24" t="s">
         <v>492</v>
       </c>
@@ -6202,7 +6202,7 @@
       </c>
       <c r="D183" s="225"/>
     </row>
-    <row r="184" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="199" t="s">
         <v>493</v>
       </c>
@@ -6210,7 +6210,7 @@
       <c r="C184" s="199"/>
       <c r="D184" s="199"/>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="24" t="s">
         <v>502</v>
       </c>
@@ -6222,7 +6222,7 @@
       </c>
       <c r="D185" s="226"/>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="24" t="s">
         <v>503</v>
       </c>
@@ -6234,7 +6234,7 @@
       </c>
       <c r="D186" s="227"/>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="24" t="s">
         <v>504</v>
       </c>
@@ -6246,7 +6246,7 @@
       </c>
       <c r="D187" s="228"/>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="24" t="s">
         <v>505</v>
       </c>
@@ -6258,7 +6258,7 @@
       </c>
       <c r="D188" s="229"/>
     </row>
-    <row r="189" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="199" t="s">
         <v>526</v>
       </c>
@@ -6266,7 +6266,7 @@
       <c r="C189" s="199"/>
       <c r="D189" s="199"/>
     </row>
-    <row r="190" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="24" t="s">
         <v>535</v>
       </c>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="D190" s="239"/>
     </row>
-    <row r="191" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="24" t="s">
         <v>536</v>
       </c>
@@ -6290,7 +6290,7 @@
       </c>
       <c r="D191" s="235"/>
     </row>
-    <row r="192" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="24" t="s">
         <v>537</v>
       </c>
@@ -6302,7 +6302,7 @@
       </c>
       <c r="D192" s="236"/>
     </row>
-    <row r="193" spans="1:4" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="24" t="s">
         <v>538</v>
       </c>
@@ -6314,7 +6314,7 @@
       </c>
       <c r="D193" s="237"/>
     </row>
-    <row r="194" spans="1:4" ht="21" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A194" s="24" t="s">
         <v>539</v>
       </c>
@@ -6326,7 +6326,7 @@
       </c>
       <c r="D194" s="238"/>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="24" t="s">
         <v>540</v>
       </c>
@@ -6352,17 +6352,17 @@
       <selection activeCell="I95" sqref="I95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" customWidth="1"/>
-    <col min="15" max="15" width="19.83203125" customWidth="1"/>
-    <col min="18" max="18" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="15" max="15" width="19.85546875" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" s="212" t="s">
         <v>456</v>
       </c>
@@ -6373,7 +6373,7 @@
       <c r="F1" s="213"/>
       <c r="G1" s="214"/>
     </row>
-    <row r="6" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>414</v>
       </c>
@@ -6408,7 +6408,7 @@
       </c>
       <c r="O6" s="6"/>
     </row>
-    <row r="7" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>415</v>
       </c>
@@ -6443,7 +6443,7 @@
       </c>
       <c r="O7" s="10"/>
     </row>
-    <row r="8" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>416</v>
       </c>
@@ -6478,31 +6478,31 @@
       </c>
       <c r="O8" s="14"/>
     </row>
-    <row r="10" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:27" x14ac:dyDescent="0.25">
       <c r="W10" s="196"/>
       <c r="X10" s="196"/>
       <c r="Y10" s="196"/>
       <c r="Z10" s="196"/>
     </row>
-    <row r="11" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:27" x14ac:dyDescent="0.25">
       <c r="W11" s="196"/>
       <c r="X11" s="196"/>
       <c r="Y11" s="196"/>
       <c r="Z11" s="196"/>
     </row>
-    <row r="12" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:27" x14ac:dyDescent="0.25">
       <c r="W12" s="196"/>
       <c r="X12" s="196"/>
       <c r="Y12" s="196"/>
       <c r="Z12" s="196"/>
     </row>
-    <row r="13" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:27" x14ac:dyDescent="0.25">
       <c r="W13" s="196"/>
       <c r="X13" s="196"/>
       <c r="Y13" s="196"/>
       <c r="Z13" s="196"/>
     </row>
-    <row r="14" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="24" t="s">
         <v>79</v>
       </c>
@@ -6524,7 +6524,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="15" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="24" t="s">
         <v>94</v>
       </c>
@@ -6546,7 +6546,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="16" spans="3:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="24" t="s">
         <v>6</v>
       </c>
@@ -6568,7 +6568,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="24" t="s">
         <v>191</v>
       </c>
@@ -6600,7 +6600,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H18" s="24" t="s">
         <v>160</v>
       </c>
@@ -6624,7 +6624,7 @@
       <c r="Y18" s="196"/>
       <c r="Z18" s="196"/>
     </row>
-    <row r="19" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H19" s="24" t="s">
         <v>191</v>
       </c>
@@ -6648,7 +6648,7 @@
       <c r="Y19" s="196"/>
       <c r="Z19" s="196"/>
     </row>
-    <row r="20" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H20" s="24" t="s">
         <v>202</v>
       </c>
@@ -6672,7 +6672,7 @@
       <c r="Y20" s="196"/>
       <c r="Z20" s="196"/>
     </row>
-    <row r="21" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="24" t="s">
         <v>75</v>
       </c>
@@ -6695,7 +6695,7 @@
       <c r="Y21" s="196"/>
       <c r="Z21" s="196"/>
     </row>
-    <row r="22" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="24" t="s">
         <v>79</v>
       </c>
@@ -6711,7 +6711,7 @@
       <c r="Y22" s="196"/>
       <c r="Z22" s="196"/>
     </row>
-    <row r="23" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="24" t="s">
         <v>191</v>
       </c>
@@ -6726,7 +6726,7 @@
       <c r="I23" s="24"/>
       <c r="J23" s="170"/>
     </row>
-    <row r="24" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="24" t="s">
         <v>186</v>
       </c>
@@ -6741,41 +6741,41 @@
       <c r="I24" s="24"/>
       <c r="J24" s="170"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="H25" s="24"/>
       <c r="I25" s="24"/>
       <c r="J25" s="170"/>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="H26" s="24"/>
       <c r="I26" s="24"/>
       <c r="J26" s="170"/>
     </row>
-    <row r="27" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="24" t="s">
         <v>88</v>
       </c>
       <c r="D27" s="62"/>
     </row>
-    <row r="28" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="24" t="s">
         <v>111</v>
       </c>
       <c r="D28" s="72"/>
     </row>
-    <row r="29" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="24" t="s">
         <v>180</v>
       </c>
       <c r="D29" s="35"/>
     </row>
-    <row r="30" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="24" t="s">
         <v>191</v>
       </c>
       <c r="D30" s="40"/>
     </row>
-    <row r="32" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>120</v>
       </c>
@@ -6794,7 +6794,7 @@
       </c>
       <c r="N32" s="77"/>
     </row>
-    <row r="33" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="24" t="s">
         <v>122</v>
       </c>
@@ -6816,7 +6816,7 @@
       </c>
       <c r="N33" s="82"/>
     </row>
-    <row r="34" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>124</v>
       </c>
@@ -6838,7 +6838,7 @@
       </c>
       <c r="N34" s="83"/>
     </row>
-    <row r="35" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="24" t="s">
         <v>128</v>
       </c>
@@ -6860,7 +6860,7 @@
       </c>
       <c r="N35" s="38"/>
     </row>
-    <row r="36" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="24" t="s">
         <v>135</v>
       </c>
@@ -6878,7 +6878,7 @@
       </c>
       <c r="N36" s="40"/>
     </row>
-    <row r="37" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="24" t="s">
         <v>137</v>
       </c>
@@ -6892,13 +6892,13 @@
       </c>
       <c r="N37" s="43"/>
     </row>
-    <row r="38" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="24" t="s">
         <v>147</v>
       </c>
       <c r="B38" s="89"/>
     </row>
-    <row r="40" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="24" t="s">
         <v>75</v>
       </c>
@@ -6921,7 +6921,7 @@
       <c r="M40" s="196"/>
       <c r="N40" s="196"/>
     </row>
-    <row r="41" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="24" t="s">
         <v>77</v>
       </c>
@@ -6944,7 +6944,7 @@
       <c r="M41" s="68"/>
       <c r="N41" s="196"/>
     </row>
-    <row r="42" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="24" t="s">
         <v>191</v>
       </c>
@@ -6967,7 +6967,7 @@
       <c r="M42" s="65"/>
       <c r="N42" s="196"/>
     </row>
-    <row r="43" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F43" s="24" t="s">
         <v>165</v>
       </c>
@@ -6977,52 +6977,52 @@
       <c r="N43" s="196"/>
       <c r="Q43" s="170"/>
     </row>
-    <row r="44" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L44" s="196"/>
       <c r="M44" s="43"/>
       <c r="N44" s="196"/>
       <c r="Q44" s="170"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L45" s="196"/>
       <c r="M45" s="196"/>
       <c r="N45" s="196"/>
       <c r="Q45" s="170"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E47" s="170"/>
     </row>
-    <row r="48" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="24" t="s">
         <v>137</v>
       </c>
       <c r="D48" s="83"/>
     </row>
-    <row r="49" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="24" t="s">
         <v>79</v>
       </c>
       <c r="D49" s="59"/>
     </row>
-    <row r="50" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C50" s="24" t="s">
         <v>94</v>
       </c>
       <c r="D50" s="151"/>
     </row>
-    <row r="51" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="24" t="s">
         <v>6</v>
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="24" t="s">
         <v>191</v>
       </c>
       <c r="D52" s="40"/>
     </row>
-    <row r="53" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="24" t="s">
         <v>52</v>
       </c>
@@ -7032,7 +7032,7 @@
       </c>
       <c r="G53" s="23"/>
     </row>
-    <row r="54" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="24" t="s">
         <v>66</v>
       </c>
@@ -7042,7 +7042,7 @@
       </c>
       <c r="G54" s="29"/>
     </row>
-    <row r="55" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C55" s="24" t="s">
         <v>167</v>
       </c>
@@ -7053,7 +7053,7 @@
       <c r="G55" s="28"/>
       <c r="H55" s="170"/>
     </row>
-    <row r="56" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C56" s="24" t="s">
         <v>70</v>
       </c>
@@ -7061,7 +7061,7 @@
       <c r="F56" s="24"/>
       <c r="H56" s="170"/>
     </row>
-    <row r="57" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C57" s="24" t="s">
         <v>147</v>
       </c>
@@ -7075,7 +7075,7 @@
       </c>
       <c r="L57" s="8"/>
     </row>
-    <row r="58" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C58" s="24" t="s">
         <v>124</v>
       </c>
@@ -7090,7 +7090,7 @@
       <c r="L58" s="14"/>
       <c r="M58" s="170"/>
     </row>
-    <row r="59" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K59" s="24" t="s">
         <v>191</v>
       </c>
@@ -7100,7 +7100,7 @@
       </c>
       <c r="P59" s="40"/>
     </row>
-    <row r="60" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C60" s="180" t="s">
         <v>417</v>
       </c>
@@ -7117,7 +7117,7 @@
       </c>
       <c r="P60" s="8"/>
     </row>
-    <row r="61" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C61" s="24" t="s">
         <v>167</v>
       </c>
@@ -7139,7 +7139,7 @@
       </c>
       <c r="P61" s="59"/>
     </row>
-    <row r="62" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C62" s="24" t="s">
         <v>139</v>
       </c>
@@ -7156,7 +7156,7 @@
       </c>
       <c r="P62" s="65"/>
     </row>
-    <row r="63" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C63" s="24" t="s">
         <v>94</v>
       </c>
@@ -7166,7 +7166,7 @@
       </c>
       <c r="M63" s="170"/>
     </row>
-    <row r="64" spans="3:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C64" s="24" t="s">
         <v>191</v>
       </c>
@@ -7175,13 +7175,13 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="65" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I65" s="24" t="s">
         <v>147</v>
       </c>
       <c r="J65" s="89"/>
     </row>
-    <row r="66" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C66" s="24" t="s">
         <v>70</v>
       </c>
@@ -7192,7 +7192,7 @@
       </c>
       <c r="J66" s="84"/>
     </row>
-    <row r="67" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C67" s="24" t="s">
         <v>147</v>
       </c>
@@ -7203,7 +7203,7 @@
       </c>
       <c r="J67" s="151"/>
     </row>
-    <row r="68" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C68" s="24" t="s">
         <v>52</v>
       </c>
@@ -7218,7 +7218,7 @@
       </c>
       <c r="P68" s="54"/>
     </row>
-    <row r="69" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I69" s="24" t="s">
         <v>196</v>
       </c>
@@ -7234,7 +7234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I70" s="24" t="s">
         <v>191</v>
       </c>
@@ -7252,7 +7252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L71" s="24" t="s">
         <v>137</v>
       </c>
@@ -7261,7 +7261,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F72" s="24" t="s">
         <v>6</v>
       </c>
@@ -7278,7 +7278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F73" s="24" t="s">
         <v>139</v>
       </c>
@@ -7295,7 +7295,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F74" s="24" t="s">
         <v>94</v>
       </c>
@@ -7312,13 +7312,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L75" s="24" t="s">
         <v>191</v>
       </c>
       <c r="M75" s="40"/>
     </row>
-    <row r="76" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L76" s="24" t="s">
         <v>99</v>
       </c>
@@ -7327,7 +7327,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="77" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G77" s="24" t="s">
         <v>67</v>
       </c>
@@ -7340,7 +7340,7 @@
       </c>
       <c r="P77" s="83"/>
     </row>
-    <row r="78" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F78" s="24" t="s">
         <v>66</v>
       </c>
@@ -7360,7 +7360,7 @@
       </c>
       <c r="P78" s="77"/>
     </row>
-    <row r="79" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F79" s="24" t="s">
         <v>188</v>
       </c>
@@ -7377,7 +7377,7 @@
       </c>
       <c r="P79" s="80"/>
     </row>
-    <row r="80" spans="3:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L80" s="24" t="s">
         <v>261</v>
       </c>
@@ -7387,7 +7387,7 @@
       </c>
       <c r="P80" s="54"/>
     </row>
-    <row r="81" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="184" t="s">
         <v>253</v>
       </c>
@@ -7417,7 +7417,7 @@
       </c>
       <c r="P81" s="52"/>
     </row>
-    <row r="82" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="187" t="s">
         <v>188</v>
       </c>
@@ -7447,7 +7447,7 @@
       </c>
       <c r="P82" s="151"/>
     </row>
-    <row r="83" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B83" s="188" t="s">
         <v>196</v>
       </c>
@@ -7477,7 +7477,7 @@
       </c>
       <c r="P83" s="66"/>
     </row>
-    <row r="84" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L84" s="24" t="s">
         <v>17</v>
       </c>
@@ -7487,7 +7487,7 @@
       </c>
       <c r="P84" s="15"/>
     </row>
-    <row r="85" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B85" s="183" t="s">
         <v>422</v>
       </c>
@@ -7500,7 +7500,7 @@
       </c>
       <c r="P85" s="9"/>
     </row>
-    <row r="86" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="24" t="s">
         <v>66</v>
       </c>
@@ -7520,7 +7520,7 @@
       </c>
       <c r="P86" s="23"/>
     </row>
-    <row r="87" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B87" s="24" t="s">
         <v>97</v>
       </c>
@@ -7540,7 +7540,7 @@
       </c>
       <c r="P87" s="40"/>
     </row>
-    <row r="88" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B88" s="24" t="s">
         <v>141</v>
       </c>
@@ -7556,7 +7556,7 @@
       </c>
       <c r="P88" s="43"/>
     </row>
-    <row r="89" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B89" s="24" t="s">
         <v>8</v>
       </c>
@@ -7572,7 +7572,7 @@
       </c>
       <c r="P89" s="127"/>
     </row>
-    <row r="90" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B90" s="24" t="s">
         <v>188</v>
       </c>
@@ -7584,7 +7584,7 @@
       </c>
       <c r="E90" s="39"/>
     </row>
-    <row r="91" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B91" s="24" t="s">
         <v>253</v>
       </c>
@@ -7596,7 +7596,7 @@
       </c>
       <c r="E91" s="88"/>
     </row>
-    <row r="92" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B92" s="24" t="s">
         <v>196</v>
       </c>
@@ -7608,7 +7608,7 @@
       </c>
       <c r="E92" s="43"/>
     </row>
-    <row r="93" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B93" s="24" t="s">
         <v>79</v>
       </c>
@@ -7620,7 +7620,7 @@
       </c>
       <c r="E93" s="59"/>
     </row>
-    <row r="94" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B94" s="24" t="s">
         <v>62</v>
       </c>
@@ -7632,167 +7632,167 @@
       </c>
       <c r="E94" s="52"/>
     </row>
-    <row r="122" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E122" s="24"/>
       <c r="F122" s="24"/>
       <c r="G122" s="170"/>
     </row>
-    <row r="123" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E123" s="24"/>
       <c r="F123" s="24"/>
       <c r="G123" s="170"/>
     </row>
-    <row r="124" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E124" s="24"/>
       <c r="F124" s="24"/>
       <c r="G124" s="170"/>
     </row>
-    <row r="125" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E125" s="24"/>
       <c r="F125" s="24"/>
       <c r="G125" s="170"/>
     </row>
-    <row r="130" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="130" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I130" s="24"/>
       <c r="J130" s="170"/>
     </row>
-    <row r="131" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="131" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I131" s="24"/>
       <c r="J131" s="170"/>
     </row>
-    <row r="132" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="132" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I132" s="24"/>
       <c r="J132" s="170"/>
     </row>
-    <row r="133" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="133" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I133" s="24"/>
       <c r="J133" s="170"/>
     </row>
-    <row r="134" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="134" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I134" s="24"/>
       <c r="J134" s="170"/>
     </row>
-    <row r="135" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="135" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I135" s="24"/>
       <c r="J135" s="170"/>
     </row>
-    <row r="136" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="136" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I136" s="24"/>
       <c r="J136" s="170"/>
     </row>
-    <row r="137" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="137" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I137" s="24"/>
       <c r="J137" s="207"/>
     </row>
-    <row r="138" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="138" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I138" s="24"/>
       <c r="J138" s="207"/>
     </row>
-    <row r="139" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="139" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I139" s="24"/>
       <c r="J139" s="207"/>
     </row>
-    <row r="140" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="140" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I140" s="24"/>
       <c r="J140" s="170"/>
     </row>
-    <row r="141" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="141" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I141" s="24"/>
       <c r="J141" s="170"/>
     </row>
-    <row r="142" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="142" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I142" s="24"/>
       <c r="J142" s="170"/>
     </row>
-    <row r="143" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="143" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I143" s="24"/>
       <c r="J143" s="170"/>
     </row>
-    <row r="144" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="144" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I144" s="24"/>
       <c r="J144" s="170"/>
     </row>
-    <row r="145" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="145" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I145" s="24"/>
       <c r="J145" s="170"/>
     </row>
-    <row r="146" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="146" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I146" s="24"/>
       <c r="J146" s="170"/>
     </row>
-    <row r="147" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="147" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I147" s="24"/>
       <c r="J147" s="170"/>
     </row>
-    <row r="148" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="148" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I148" s="24"/>
       <c r="J148" s="170"/>
     </row>
-    <row r="149" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="149" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I149" s="24"/>
       <c r="J149" s="170"/>
     </row>
-    <row r="150" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="150" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I150" s="24"/>
       <c r="J150" s="170"/>
     </row>
-    <row r="151" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="151" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I151" s="24"/>
       <c r="J151" s="170"/>
     </row>
-    <row r="152" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="152" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I152" s="24"/>
       <c r="J152" s="24"/>
     </row>
-    <row r="153" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="153" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I153" s="24"/>
       <c r="J153" s="24"/>
     </row>
-    <row r="154" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="154" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I154" s="24"/>
       <c r="J154" s="24"/>
     </row>
-    <row r="155" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="155" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I155" s="24"/>
       <c r="J155" s="24"/>
     </row>
-    <row r="156" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="156" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I156" s="24"/>
       <c r="J156" s="170"/>
     </row>
-    <row r="157" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="157" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I157" s="24"/>
       <c r="J157" s="24"/>
     </row>
-    <row r="158" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="158" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I158" s="24"/>
       <c r="J158" s="24"/>
     </row>
-    <row r="159" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="159" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I159" s="24"/>
       <c r="J159" s="24"/>
     </row>
-    <row r="160" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="160" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I160" s="24"/>
       <c r="J160" s="170"/>
     </row>
-    <row r="161" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="161" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I161" s="24"/>
       <c r="J161" s="170"/>
     </row>
-    <row r="162" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="162" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I162" s="24"/>
       <c r="J162" s="170"/>
     </row>
-    <row r="163" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="163" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I163" s="24"/>
       <c r="J163" s="170"/>
     </row>
-    <row r="164" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="164" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I164" s="24"/>
       <c r="J164" s="170"/>
     </row>
-    <row r="165" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="165" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I165" s="24"/>
       <c r="J165" s="170"/>
     </row>

</xml_diff>